<commit_message>
added author's photos + fixed login.html and registration.html
</commit_message>
<xml_diff>
--- a/Schedule_maker/static/xlsx/schedule.xlsx
+++ b/Schedule_maker/static/xlsx/schedule.xlsx
@@ -77,7 +77,7 @@
     <t>Алгоритмы и структуры данных</t>
   </si>
   <si>
-    <t>Kaitlyn Allen</t>
+    <t>Jeffrey Perez</t>
   </si>
   <si>
     <t>306</t>
@@ -86,49 +86,52 @@
     <t>math</t>
   </si>
   <si>
-    <t>Victoria Baker</t>
+    <t>Stephen Bennett</t>
   </si>
   <si>
     <t>science</t>
   </si>
   <si>
-    <t>Erica Romero</t>
+    <t>Darryl Rivas</t>
   </si>
   <si>
     <t>geography</t>
   </si>
   <si>
-    <t>Marie Petersen</t>
+    <t>Heather Reyes</t>
   </si>
   <si>
     <t>I.T.</t>
   </si>
   <si>
-    <t>Emily Smith</t>
+    <t>John Lawson</t>
   </si>
   <si>
     <t>biology</t>
   </si>
   <si>
-    <t>Steven Hunter</t>
+    <t>Eric Payne</t>
   </si>
   <si>
     <t>105</t>
   </si>
   <si>
-    <t>Raymond Robinson</t>
+    <t>Robert Preston</t>
   </si>
   <si>
     <t>325</t>
   </si>
   <si>
+    <t>Allison Martinez</t>
+  </si>
+  <si>
+    <t>Taylor Ingram</t>
+  </si>
+  <si>
     <t>313</t>
   </si>
   <si>
-    <t>Scott Pollard</t>
-  </si>
-  <si>
-    <t>Betty Newman</t>
+    <t>David Gibbs</t>
   </si>
   <si>
     <t>329</t>
@@ -137,22 +140,19 @@
     <t>326</t>
   </si>
   <si>
-    <t>Daniel Fowler</t>
+    <t>James Roberts</t>
   </si>
   <si>
     <t>407</t>
   </si>
   <si>
+    <t>Jason Gentry</t>
+  </si>
+  <si>
     <t>420</t>
   </si>
   <si>
-    <t>Christopher Stewart</t>
-  </si>
-  <si>
     <t>327</t>
-  </si>
-  <si>
-    <t>Ashley Gross</t>
   </si>
   <si>
     <t>507</t>
@@ -161,49 +161,52 @@
     <t>art</t>
   </si>
   <si>
-    <t>Patricia Odom</t>
+    <t>Alex Hawkins</t>
   </si>
   <si>
     <t>history</t>
   </si>
   <si>
-    <t>William Duncan</t>
+    <t>Ricky Morales</t>
   </si>
   <si>
     <t>music</t>
   </si>
   <si>
-    <t>Daniel Diaz</t>
+    <t>James Bauer</t>
   </si>
   <si>
     <t>P.E.</t>
   </si>
   <si>
-    <t>Eric Butler</t>
+    <t>Karen Huff</t>
   </si>
   <si>
-    <t>Denise Bowman</t>
+    <t>Steven Swanson</t>
+  </si>
+  <si>
+    <t>Jessica Wolf</t>
   </si>
   <si>
     <t>116</t>
   </si>
   <si>
-    <t>Aaron Maddox</t>
-  </si>
-  <si>
-    <t>James Miller</t>
-  </si>
-  <si>
-    <t>Gregory Hendricks</t>
+    <t>Rebecca Delacruz</t>
   </si>
   <si>
     <t>107</t>
   </si>
   <si>
+    <t>Linda Long</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10702122 10702222</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 10702322 10702422</t>
   </si>
   <si>
-    <t xml:space="preserve"> 10702322</t>
+    <t xml:space="preserve"> 10702422</t>
   </si>
   <si>
     <t xml:space="preserve"> 10701222</t>
@@ -212,22 +215,19 @@
     <t xml:space="preserve"> 10701322</t>
   </si>
   <si>
+    <t xml:space="preserve"> 10701122 10701222 10701322</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10702322</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10701122</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 10702122</t>
   </si>
   <si>
     <t xml:space="preserve"> 10702222</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 10701122 10701222 10701322</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 10702122 10702222</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 10702422</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 10701122</t>
   </si>
   <si>
     <t xml:space="preserve"> 10702122 10702222 10702322 10702422</t>
@@ -820,13 +820,13 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
@@ -870,13 +870,13 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
@@ -902,7 +902,7 @@
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
@@ -973,16 +973,16 @@
         <v>20</v>
       </c>
       <c r="D22" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="G22" s="8" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="5" t="s">
@@ -1005,16 +1005,16 @@
         <v>32</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H23" s="9"/>
       <c r="I23" s="6" t="s">
@@ -1040,7 +1040,7 @@
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10" t="s">
@@ -1086,15 +1086,15 @@
       <c r="A26" s="2"/>
       <c r="B26" s="1"/>
       <c r="C26" s="11" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="11" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="H26" s="11"/>
       <c r="I26" s="11" t="s">
@@ -1118,15 +1118,15 @@
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J27" s="12"/>
       <c r="K27" s="9"/>
@@ -1238,13 +1238,13 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
@@ -1288,13 +1288,13 @@
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
       <c r="M34" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
@@ -1320,7 +1320,7 @@
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
       <c r="M35" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
@@ -1342,7 +1342,9 @@
       <c r="E36" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F36" s="7"/>
+      <c r="F36" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="G36" s="7" t="s">
         <v>24</v>
       </c>
@@ -1353,10 +1355,10 @@
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
-      <c r="M36" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="N36" s="7"/>
+      <c r="M36" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N36" s="10"/>
       <c r="O36" s="10" t="s">
         <v>22</v>
       </c>
@@ -1379,8 +1381,8 @@
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
-      <c r="M37" s="7"/>
-      <c r="N37" s="7"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
       <c r="O37" s="10"/>
       <c r="P37" s="10"/>
       <c r="Q37" s="1"/>
@@ -1393,28 +1395,30 @@
         <v>20</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F38" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="G38" s="8" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="H38" s="9"/>
       <c r="I38" s="5" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
-      <c r="M38" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N38" s="9"/>
+      <c r="M38" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N38" s="11"/>
       <c r="O38" s="11" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="P38" s="11"/>
       <c r="Q38" s="1"/>
@@ -1427,14 +1431,16 @@
         <v>32</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F39" s="9"/>
+        <v>39</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="G39" s="9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H39" s="9"/>
       <c r="I39" s="6" t="s">
@@ -1443,12 +1449,12 @@
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
-      <c r="M39" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="N39" s="9"/>
+      <c r="M39" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="N39" s="12"/>
       <c r="O39" s="12" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="P39" s="12"/>
       <c r="Q39" s="1"/>
@@ -1461,24 +1467,24 @@
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
-      <c r="E40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F40" s="10"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
       <c r="G40" s="10" t="s">
         <v>26</v>
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="10" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="J40" s="10"/>
       <c r="K40" s="10" t="s">
         <v>22</v>
       </c>
       <c r="L40" s="10"/>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
+      <c r="M40" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="N40" s="10"/>
       <c r="O40" s="7"/>
       <c r="P40" s="7"/>
       <c r="Q40" s="1" t="s">
@@ -1491,16 +1497,16 @@
       <c r="B41" s="1"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
       <c r="I41" s="10"/>
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
       <c r="L41" s="10"/>
-      <c r="M41" s="7"/>
-      <c r="N41" s="7"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
       <c r="O41" s="7"/>
       <c r="P41" s="7"/>
       <c r="Q41" s="1"/>
@@ -1511,24 +1517,24 @@
       <c r="B42" s="1"/>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
-      <c r="E42" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F42" s="11"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
       <c r="G42" s="11" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="H42" s="11"/>
       <c r="I42" s="11" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="J42" s="11"/>
       <c r="K42" s="11" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="L42" s="11"/>
-      <c r="M42" s="9"/>
-      <c r="N42" s="9"/>
+      <c r="M42" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="N42" s="11"/>
       <c r="O42" s="9"/>
       <c r="P42" s="9"/>
       <c r="Q42" s="1"/>
@@ -1539,24 +1545,24 @@
       <c r="B43" s="1"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="12" t="s">
         <v>34</v>
-      </c>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12" t="s">
-        <v>39</v>
       </c>
       <c r="H43" s="12"/>
       <c r="I43" s="12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J43" s="12"/>
       <c r="K43" s="12" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="L43" s="12"/>
-      <c r="M43" s="9"/>
-      <c r="N43" s="9"/>
+      <c r="M43" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="N43" s="12"/>
       <c r="O43" s="9"/>
       <c r="P43" s="9"/>
       <c r="Q43" s="1"/>
@@ -1662,7 +1668,7 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
@@ -1712,7 +1718,7 @@
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
       <c r="I50" s="5" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
@@ -1744,7 +1750,7 @@
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
       <c r="M51" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N51" s="6"/>
       <c r="O51" s="6"/>
@@ -1761,30 +1767,30 @@
         <v>22</v>
       </c>
       <c r="D52" s="10"/>
-      <c r="E52" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F52" s="7"/>
+      <c r="E52" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F52" s="10"/>
       <c r="G52" s="7" t="s">
         <v>19</v>
       </c>
       <c r="H52" s="7"/>
       <c r="I52" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J52" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="J52" s="7"/>
-      <c r="K52" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="L52" s="7"/>
-      <c r="M52" s="10" t="s">
+      <c r="K52" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="N52" s="10"/>
-      <c r="O52" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="P52" s="10"/>
+      <c r="L52" s="10"/>
+      <c r="M52" s="7"/>
+      <c r="N52" s="7"/>
+      <c r="O52" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="P52" s="7"/>
       <c r="Q52" s="1" t="s">
         <v>9</v>
       </c>
@@ -1795,18 +1801,18 @@
       <c r="B53" s="1"/>
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
       <c r="J53" s="7"/>
-      <c r="K53" s="7"/>
-      <c r="L53" s="7"/>
-      <c r="M53" s="10"/>
-      <c r="N53" s="10"/>
-      <c r="O53" s="10"/>
-      <c r="P53" s="10"/>
+      <c r="K53" s="10"/>
+      <c r="L53" s="10"/>
+      <c r="M53" s="7"/>
+      <c r="N53" s="7"/>
+      <c r="O53" s="7"/>
+      <c r="P53" s="7"/>
       <c r="Q53" s="1"/>
       <c r="R53" s="4"/>
     </row>
@@ -1817,30 +1823,30 @@
         <v>33</v>
       </c>
       <c r="D54" s="11"/>
-      <c r="E54" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F54" s="9"/>
+      <c r="E54" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F54" s="11"/>
       <c r="G54" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H54" s="9"/>
       <c r="I54" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J54" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="J54" s="9"/>
-      <c r="K54" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="L54" s="9"/>
-      <c r="M54" s="11" t="s">
+      <c r="K54" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="L54" s="11"/>
+      <c r="M54" s="9"/>
+      <c r="N54" s="9"/>
+      <c r="O54" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="N54" s="11"/>
-      <c r="O54" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="P54" s="11"/>
+      <c r="P54" s="9"/>
       <c r="Q54" s="1"/>
       <c r="R54" s="4"/>
     </row>
@@ -1851,30 +1857,30 @@
         <v>34</v>
       </c>
       <c r="D55" s="12"/>
-      <c r="E55" s="9" t="s">
+      <c r="E55" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F55" s="12"/>
+      <c r="G55" s="9" t="s">
         <v>32</v>
-      </c>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9" t="s">
-        <v>35</v>
       </c>
       <c r="H55" s="9"/>
       <c r="I55" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="J55" s="9"/>
-      <c r="K55" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="L55" s="9"/>
-      <c r="M55" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="J55" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N55" s="12"/>
-      <c r="O55" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="P55" s="12"/>
+      <c r="K55" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="L55" s="12"/>
+      <c r="M55" s="9"/>
+      <c r="N55" s="9"/>
+      <c r="O55" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P55" s="9"/>
       <c r="Q55" s="1"/>
       <c r="R55" s="4"/>
     </row>
@@ -1891,20 +1897,20 @@
         <v>30</v>
       </c>
       <c r="H56" s="10"/>
-      <c r="I56" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J56" s="10"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
       <c r="K56" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L56" s="10"/>
       <c r="M56" s="10" t="s">
         <v>22</v>
       </c>
       <c r="N56" s="10"/>
-      <c r="O56" s="7"/>
-      <c r="P56" s="7"/>
+      <c r="O56" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P56" s="10"/>
       <c r="Q56" s="1" t="s">
         <v>10</v>
       </c>
@@ -1919,14 +1925,14 @@
       <c r="F57" s="7"/>
       <c r="G57" s="10"/>
       <c r="H57" s="10"/>
-      <c r="I57" s="10"/>
-      <c r="J57" s="10"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7"/>
       <c r="K57" s="10"/>
       <c r="L57" s="10"/>
       <c r="M57" s="10"/>
       <c r="N57" s="10"/>
-      <c r="O57" s="7"/>
-      <c r="P57" s="7"/>
+      <c r="O57" s="10"/>
+      <c r="P57" s="10"/>
       <c r="Q57" s="1"/>
       <c r="R57" s="4"/>
     </row>
@@ -1938,23 +1944,23 @@
       <c r="E58" s="9"/>
       <c r="F58" s="9"/>
       <c r="G58" s="11" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="H58" s="11"/>
-      <c r="I58" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="J58" s="11"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
       <c r="K58" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L58" s="11"/>
       <c r="M58" s="11" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="N58" s="11"/>
-      <c r="O58" s="9"/>
-      <c r="P58" s="9"/>
+      <c r="O58" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="P58" s="11"/>
       <c r="Q58" s="1"/>
       <c r="R58" s="4"/>
     </row>
@@ -1969,20 +1975,20 @@
         <v>34</v>
       </c>
       <c r="H59" s="12"/>
-      <c r="I59" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="J59" s="12"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="9"/>
       <c r="K59" s="12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="L59" s="12"/>
       <c r="M59" s="12" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="N59" s="12"/>
-      <c r="O59" s="9"/>
-      <c r="P59" s="9"/>
+      <c r="O59" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="P59" s="12"/>
       <c r="Q59" s="1"/>
       <c r="R59" s="4"/>
     </row>
@@ -2142,7 +2148,7 @@
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
       <c r="M66" s="5" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="N66" s="5"/>
       <c r="O66" s="5"/>
@@ -2168,7 +2174,7 @@
       <c r="K67" s="6"/>
       <c r="L67" s="6"/>
       <c r="M67" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N67" s="6"/>
       <c r="O67" s="6"/>
@@ -2197,14 +2203,18 @@
         <v>47</v>
       </c>
       <c r="J68" s="10"/>
-      <c r="K68" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="L68" s="10"/>
+      <c r="K68" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L68" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="M68" s="7"/>
       <c r="N68" s="7"/>
-      <c r="O68" s="7"/>
-      <c r="P68" s="7"/>
+      <c r="O68" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P68" s="10"/>
       <c r="Q68" s="1" t="s">
         <v>9</v>
       </c>
@@ -2221,12 +2231,12 @@
       <c r="H69" s="7"/>
       <c r="I69" s="10"/>
       <c r="J69" s="10"/>
-      <c r="K69" s="10"/>
-      <c r="L69" s="10"/>
+      <c r="K69" s="7"/>
+      <c r="L69" s="7"/>
       <c r="M69" s="7"/>
       <c r="N69" s="7"/>
-      <c r="O69" s="7"/>
-      <c r="P69" s="7"/>
+      <c r="O69" s="10"/>
+      <c r="P69" s="10"/>
       <c r="Q69" s="1"/>
       <c r="R69" s="4"/>
     </row>
@@ -2242,21 +2252,25 @@
       </c>
       <c r="F70" s="11"/>
       <c r="G70" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H70" s="9"/>
       <c r="I70" s="11" t="s">
         <v>55</v>
       </c>
       <c r="J70" s="11"/>
-      <c r="K70" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="L70" s="11"/>
+      <c r="K70" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L70" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="M70" s="9"/>
       <c r="N70" s="9"/>
-      <c r="O70" s="9"/>
-      <c r="P70" s="9"/>
+      <c r="O70" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="P70" s="11"/>
       <c r="Q70" s="1"/>
       <c r="R70" s="4"/>
     </row>
@@ -2268,7 +2282,7 @@
       </c>
       <c r="D71" s="12"/>
       <c r="E71" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F71" s="12"/>
       <c r="G71" s="9" t="s">
@@ -2276,17 +2290,21 @@
       </c>
       <c r="H71" s="9"/>
       <c r="I71" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J71" s="12"/>
-      <c r="K71" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="L71" s="12"/>
+      <c r="K71" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="L71" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="M71" s="9"/>
       <c r="N71" s="9"/>
-      <c r="O71" s="9"/>
-      <c r="P71" s="9"/>
+      <c r="O71" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="P71" s="12"/>
       <c r="Q71" s="1"/>
       <c r="R71" s="4"/>
     </row>
@@ -2304,13 +2322,11 @@
       <c r="I72" s="7"/>
       <c r="J72" s="7"/>
       <c r="K72" s="10" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="L72" s="10"/>
-      <c r="M72" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="N72" s="10"/>
+      <c r="M72" s="7"/>
+      <c r="N72" s="7"/>
       <c r="O72" s="7"/>
       <c r="P72" s="7"/>
       <c r="Q72" s="1" t="s">
@@ -2331,8 +2347,8 @@
       <c r="J73" s="7"/>
       <c r="K73" s="10"/>
       <c r="L73" s="10"/>
-      <c r="M73" s="10"/>
-      <c r="N73" s="10"/>
+      <c r="M73" s="7"/>
+      <c r="N73" s="7"/>
       <c r="O73" s="7"/>
       <c r="P73" s="7"/>
       <c r="Q73" s="1"/>
@@ -2350,13 +2366,11 @@
       <c r="I74" s="9"/>
       <c r="J74" s="9"/>
       <c r="K74" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L74" s="11"/>
-      <c r="M74" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="N74" s="11"/>
+      <c r="M74" s="9"/>
+      <c r="N74" s="9"/>
       <c r="O74" s="9"/>
       <c r="P74" s="9"/>
       <c r="Q74" s="1"/>
@@ -2377,10 +2391,8 @@
         <v>34</v>
       </c>
       <c r="L75" s="12"/>
-      <c r="M75" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="N75" s="12"/>
+      <c r="M75" s="9"/>
+      <c r="N75" s="9"/>
       <c r="O75" s="9"/>
       <c r="P75" s="9"/>
       <c r="Q75" s="1"/>
@@ -2494,13 +2506,13 @@
       <c r="M80" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="N80" s="7"/>
+      <c r="N80" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="O80" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="P80" s="7" t="s">
-        <v>28</v>
-      </c>
+      <c r="P80" s="7"/>
       <c r="Q80" s="1" t="s">
         <v>8</v>
       </c>
@@ -2546,15 +2558,15 @@
       <c r="K82" s="5"/>
       <c r="L82" s="5"/>
       <c r="M82" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="N82" s="9"/>
+        <v>20</v>
+      </c>
+      <c r="N82" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="O82" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P82" s="8" t="s">
-        <v>36</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="P82" s="9"/>
       <c r="Q82" s="1"/>
       <c r="R82" s="4"/>
     </row>
@@ -2578,13 +2590,13 @@
       <c r="M83" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="N83" s="9"/>
+      <c r="N83" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="O83" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="P83" s="9" t="s">
-        <v>38</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="P83" s="9"/>
       <c r="Q83" s="1"/>
       <c r="R83" s="4"/>
     </row>
@@ -2598,21 +2610,19 @@
       </c>
       <c r="D84" s="10"/>
       <c r="E84" s="10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F84" s="10"/>
       <c r="G84" s="10" t="s">
         <v>22</v>
       </c>
       <c r="H84" s="10"/>
-      <c r="I84" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J84" s="7"/>
-      <c r="K84" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="L84" s="10"/>
+      <c r="I84" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J84" s="10"/>
+      <c r="K84" s="7"/>
+      <c r="L84" s="7"/>
       <c r="M84" s="7"/>
       <c r="N84" s="7"/>
       <c r="O84" s="7"/>
@@ -2631,10 +2641,10 @@
       <c r="F85" s="10"/>
       <c r="G85" s="10"/>
       <c r="H85" s="10"/>
-      <c r="I85" s="7"/>
-      <c r="J85" s="7"/>
-      <c r="K85" s="10"/>
-      <c r="L85" s="10"/>
+      <c r="I85" s="10"/>
+      <c r="J85" s="10"/>
+      <c r="K85" s="7"/>
+      <c r="L85" s="7"/>
       <c r="M85" s="7"/>
       <c r="N85" s="7"/>
       <c r="O85" s="7"/>
@@ -2646,25 +2656,23 @@
       <c r="A86" s="2"/>
       <c r="B86" s="1"/>
       <c r="C86" s="11" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D86" s="11"/>
       <c r="E86" s="11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F86" s="11"/>
       <c r="G86" s="11" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="H86" s="11"/>
-      <c r="I86" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="J86" s="9"/>
-      <c r="K86" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="L86" s="11"/>
+      <c r="I86" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J86" s="11"/>
+      <c r="K86" s="9"/>
+      <c r="L86" s="9"/>
       <c r="M86" s="9"/>
       <c r="N86" s="9"/>
       <c r="O86" s="9"/>
@@ -2680,21 +2688,19 @@
       </c>
       <c r="D87" s="12"/>
       <c r="E87" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F87" s="12"/>
       <c r="G87" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H87" s="12"/>
-      <c r="I87" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="J87" s="9"/>
-      <c r="K87" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="L87" s="12"/>
+      <c r="I87" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="J87" s="12"/>
+      <c r="K87" s="9"/>
+      <c r="L87" s="9"/>
       <c r="M87" s="9"/>
       <c r="N87" s="9"/>
       <c r="O87" s="9"/>
@@ -2715,14 +2721,14 @@
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
       <c r="J88" s="7"/>
-      <c r="K88" s="7"/>
-      <c r="L88" s="7"/>
+      <c r="K88" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L88" s="10"/>
       <c r="M88" s="7"/>
       <c r="N88" s="7"/>
-      <c r="O88" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="P88" s="10"/>
+      <c r="O88" s="7"/>
+      <c r="P88" s="7"/>
       <c r="Q88" s="1" t="s">
         <v>10</v>
       </c>
@@ -2739,12 +2745,12 @@
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
       <c r="J89" s="7"/>
-      <c r="K89" s="7"/>
-      <c r="L89" s="7"/>
+      <c r="K89" s="10"/>
+      <c r="L89" s="10"/>
       <c r="M89" s="7"/>
       <c r="N89" s="7"/>
-      <c r="O89" s="10"/>
-      <c r="P89" s="10"/>
+      <c r="O89" s="7"/>
+      <c r="P89" s="7"/>
       <c r="Q89" s="1"/>
       <c r="R89" s="4"/>
     </row>
@@ -2759,14 +2765,14 @@
       <c r="H90" s="9"/>
       <c r="I90" s="9"/>
       <c r="J90" s="9"/>
-      <c r="K90" s="9"/>
-      <c r="L90" s="9"/>
+      <c r="K90" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L90" s="11"/>
       <c r="M90" s="9"/>
       <c r="N90" s="9"/>
-      <c r="O90" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="P90" s="11"/>
+      <c r="O90" s="9"/>
+      <c r="P90" s="9"/>
       <c r="Q90" s="1"/>
       <c r="R90" s="4"/>
     </row>
@@ -2781,14 +2787,14 @@
       <c r="H91" s="9"/>
       <c r="I91" s="9"/>
       <c r="J91" s="9"/>
-      <c r="K91" s="9"/>
-      <c r="L91" s="9"/>
+      <c r="K91" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="L91" s="12"/>
       <c r="M91" s="9"/>
       <c r="N91" s="9"/>
-      <c r="O91" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="P91" s="12"/>
+      <c r="O91" s="9"/>
+      <c r="P91" s="9"/>
       <c r="Q91" s="1"/>
       <c r="R91" s="4"/>
     </row>
@@ -2986,7 +2992,7 @@
       </c>
       <c r="D100" s="10"/>
       <c r="E100" s="10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F100" s="10"/>
       <c r="G100" s="10" t="s">
@@ -2994,12 +3000,10 @@
       </c>
       <c r="H100" s="10"/>
       <c r="I100" s="10" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="J100" s="10"/>
-      <c r="K100" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="K100" s="7"/>
       <c r="L100" s="7"/>
       <c r="M100" s="7"/>
       <c r="N100" s="7"/>
@@ -3038,20 +3042,18 @@
       </c>
       <c r="D102" s="11"/>
       <c r="E102" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F102" s="11"/>
       <c r="G102" s="11" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="H102" s="11"/>
       <c r="I102" s="11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J102" s="11"/>
-      <c r="K102" s="8" t="s">
-        <v>37</v>
-      </c>
+      <c r="K102" s="9"/>
       <c r="L102" s="9"/>
       <c r="M102" s="9"/>
       <c r="N102" s="9"/>
@@ -3068,20 +3070,18 @@
       </c>
       <c r="D103" s="12"/>
       <c r="E103" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F103" s="12"/>
       <c r="G103" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H103" s="12"/>
       <c r="I103" s="12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J103" s="12"/>
-      <c r="K103" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="K103" s="9"/>
       <c r="L103" s="9"/>
       <c r="M103" s="9"/>
       <c r="N103" s="9"/>
@@ -3414,7 +3414,9 @@
     <mergeCell ref="D110:D111"/>
     <mergeCell ref="E20:E21"/>
     <mergeCell ref="E36:E37"/>
-    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="E52:F53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E55:F55"/>
     <mergeCell ref="E68:F69"/>
     <mergeCell ref="E70:F70"/>
     <mergeCell ref="E71:F71"/>
@@ -3427,9 +3429,8 @@
     <mergeCell ref="E24:F25"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E40:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="E42:E43"/>
     <mergeCell ref="E56:E57"/>
     <mergeCell ref="E58:E59"/>
     <mergeCell ref="E72:E73"/>
@@ -3452,9 +3453,8 @@
     <mergeCell ref="E110:E111"/>
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="F36:F37"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="F42:F43"/>
     <mergeCell ref="F56:F57"/>
     <mergeCell ref="F58:F59"/>
     <mergeCell ref="F72:F73"/>
@@ -3566,7 +3566,9 @@
     <mergeCell ref="I68:J69"/>
     <mergeCell ref="I70:J70"/>
     <mergeCell ref="I71:J71"/>
-    <mergeCell ref="I84:I85"/>
+    <mergeCell ref="I84:J85"/>
+    <mergeCell ref="I86:J86"/>
+    <mergeCell ref="I87:J87"/>
     <mergeCell ref="I100:J101"/>
     <mergeCell ref="I102:J102"/>
     <mergeCell ref="I103:J103"/>
@@ -3576,9 +3578,8 @@
     <mergeCell ref="I40:J41"/>
     <mergeCell ref="I42:J42"/>
     <mergeCell ref="I43:J43"/>
-    <mergeCell ref="I56:J57"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="I56:I57"/>
+    <mergeCell ref="I58:I59"/>
     <mergeCell ref="I72:I73"/>
     <mergeCell ref="I74:I75"/>
     <mergeCell ref="I88:I89"/>
@@ -3598,9 +3599,8 @@
     <mergeCell ref="I108:I109"/>
     <mergeCell ref="I110:I111"/>
     <mergeCell ref="J52:J53"/>
-    <mergeCell ref="J54:J55"/>
-    <mergeCell ref="J84:J85"/>
-    <mergeCell ref="J86:J87"/>
+    <mergeCell ref="J56:J57"/>
+    <mergeCell ref="J58:J59"/>
     <mergeCell ref="J72:J73"/>
     <mergeCell ref="J74:J75"/>
     <mergeCell ref="J88:J89"/>
@@ -3619,14 +3619,14 @@
     <mergeCell ref="J94:J95"/>
     <mergeCell ref="J108:J109"/>
     <mergeCell ref="J110:J111"/>
-    <mergeCell ref="K52:K53"/>
-    <mergeCell ref="K68:L69"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="K71:L71"/>
-    <mergeCell ref="K84:L85"/>
-    <mergeCell ref="K86:L86"/>
-    <mergeCell ref="K87:L87"/>
+    <mergeCell ref="K52:L53"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K68:K69"/>
+    <mergeCell ref="K84:K85"/>
+    <mergeCell ref="K86:K87"/>
     <mergeCell ref="K100:K101"/>
+    <mergeCell ref="K102:K103"/>
     <mergeCell ref="K24:K25"/>
     <mergeCell ref="K26:K27"/>
     <mergeCell ref="K40:L41"/>
@@ -3638,8 +3638,9 @@
     <mergeCell ref="K72:L73"/>
     <mergeCell ref="K74:L74"/>
     <mergeCell ref="K75:L75"/>
-    <mergeCell ref="K88:K89"/>
-    <mergeCell ref="K90:K91"/>
+    <mergeCell ref="K88:L89"/>
+    <mergeCell ref="K90:L90"/>
+    <mergeCell ref="K91:L91"/>
     <mergeCell ref="K104:K105"/>
     <mergeCell ref="K106:K107"/>
     <mergeCell ref="K28:K29"/>
@@ -3654,14 +3655,13 @@
     <mergeCell ref="K94:K95"/>
     <mergeCell ref="K108:K109"/>
     <mergeCell ref="K110:K111"/>
-    <mergeCell ref="L52:L53"/>
-    <mergeCell ref="L54:L55"/>
+    <mergeCell ref="L68:L69"/>
+    <mergeCell ref="L84:L85"/>
+    <mergeCell ref="L86:L87"/>
     <mergeCell ref="L100:L101"/>
     <mergeCell ref="L102:L103"/>
     <mergeCell ref="L24:L25"/>
     <mergeCell ref="L26:L27"/>
-    <mergeCell ref="L88:L89"/>
-    <mergeCell ref="L90:L91"/>
     <mergeCell ref="L104:L105"/>
     <mergeCell ref="L106:L107"/>
     <mergeCell ref="L28:L29"/>
@@ -3689,10 +3689,11 @@
     <mergeCell ref="M66:P66"/>
     <mergeCell ref="M67:P67"/>
     <mergeCell ref="M80:M81"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="M52:N53"/>
-    <mergeCell ref="M54:N54"/>
-    <mergeCell ref="M55:N55"/>
+    <mergeCell ref="M36:N37"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M52:M53"/>
+    <mergeCell ref="M54:M55"/>
     <mergeCell ref="M68:M69"/>
     <mergeCell ref="M70:M71"/>
     <mergeCell ref="M84:M85"/>
@@ -3701,14 +3702,14 @@
     <mergeCell ref="M102:M103"/>
     <mergeCell ref="M24:M25"/>
     <mergeCell ref="M26:M27"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="M42:M43"/>
+    <mergeCell ref="M40:N41"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="M43:N43"/>
     <mergeCell ref="M56:N57"/>
     <mergeCell ref="M58:N58"/>
     <mergeCell ref="M59:N59"/>
-    <mergeCell ref="M72:N73"/>
-    <mergeCell ref="M74:N74"/>
-    <mergeCell ref="M75:N75"/>
+    <mergeCell ref="M72:M73"/>
+    <mergeCell ref="M74:M75"/>
     <mergeCell ref="M88:M89"/>
     <mergeCell ref="M90:M91"/>
     <mergeCell ref="M104:M105"/>
@@ -3726,9 +3727,8 @@
     <mergeCell ref="M108:M109"/>
     <mergeCell ref="M110:M111"/>
     <mergeCell ref="N80:N81"/>
-    <mergeCell ref="N82:N83"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="N52:N53"/>
+    <mergeCell ref="N54:N55"/>
     <mergeCell ref="N68:N69"/>
     <mergeCell ref="N70:N71"/>
     <mergeCell ref="N84:N85"/>
@@ -3737,8 +3737,8 @@
     <mergeCell ref="N102:N103"/>
     <mergeCell ref="N24:N25"/>
     <mergeCell ref="N26:N27"/>
-    <mergeCell ref="N40:N41"/>
-    <mergeCell ref="N42:N43"/>
+    <mergeCell ref="N72:N73"/>
+    <mergeCell ref="N74:N75"/>
     <mergeCell ref="N88:N89"/>
     <mergeCell ref="N90:N91"/>
     <mergeCell ref="N104:N105"/>
@@ -3759,11 +3759,10 @@
     <mergeCell ref="O36:P37"/>
     <mergeCell ref="O38:P38"/>
     <mergeCell ref="O39:P39"/>
-    <mergeCell ref="O52:P53"/>
-    <mergeCell ref="O54:P54"/>
-    <mergeCell ref="O55:P55"/>
-    <mergeCell ref="O68:O69"/>
-    <mergeCell ref="O70:O71"/>
+    <mergeCell ref="O52:O53"/>
+    <mergeCell ref="O68:P69"/>
+    <mergeCell ref="O70:P70"/>
+    <mergeCell ref="O71:P71"/>
     <mergeCell ref="O84:O85"/>
     <mergeCell ref="O86:O87"/>
     <mergeCell ref="O100:O101"/>
@@ -3772,13 +3771,13 @@
     <mergeCell ref="O26:O27"/>
     <mergeCell ref="O40:O41"/>
     <mergeCell ref="O42:O43"/>
-    <mergeCell ref="O56:O57"/>
-    <mergeCell ref="O58:O59"/>
+    <mergeCell ref="O56:P57"/>
+    <mergeCell ref="O58:P58"/>
+    <mergeCell ref="O59:P59"/>
     <mergeCell ref="O72:O73"/>
     <mergeCell ref="O74:O75"/>
-    <mergeCell ref="O88:P89"/>
-    <mergeCell ref="O90:P90"/>
-    <mergeCell ref="O91:P91"/>
+    <mergeCell ref="O88:O89"/>
+    <mergeCell ref="O90:O91"/>
     <mergeCell ref="O104:O105"/>
     <mergeCell ref="O106:O107"/>
     <mergeCell ref="O28:O29"/>
@@ -3794,8 +3793,9 @@
     <mergeCell ref="O108:O109"/>
     <mergeCell ref="O110:O111"/>
     <mergeCell ref="P80:P81"/>
-    <mergeCell ref="P68:P69"/>
-    <mergeCell ref="P70:P71"/>
+    <mergeCell ref="P82:P83"/>
+    <mergeCell ref="P52:P53"/>
+    <mergeCell ref="P54:P55"/>
     <mergeCell ref="P84:P85"/>
     <mergeCell ref="P86:P87"/>
     <mergeCell ref="P100:P101"/>
@@ -3804,10 +3804,10 @@
     <mergeCell ref="P26:P27"/>
     <mergeCell ref="P40:P41"/>
     <mergeCell ref="P42:P43"/>
-    <mergeCell ref="P56:P57"/>
-    <mergeCell ref="P58:P59"/>
     <mergeCell ref="P72:P73"/>
     <mergeCell ref="P74:P75"/>
+    <mergeCell ref="P88:P89"/>
+    <mergeCell ref="P90:P91"/>
     <mergeCell ref="P104:P105"/>
     <mergeCell ref="P106:P107"/>
     <mergeCell ref="P28:P29"/>
@@ -3848,7 +3848,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
@@ -3856,15 +3856,15 @@
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1" t="s">
@@ -3876,11 +3876,11 @@
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="1" t="s">
@@ -3888,15 +3888,15 @@
       </c>
       <c r="V11" s="1"/>
       <c r="W11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X11" s="1"/>
       <c r="Y11" s="1" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1" t="s">
@@ -3904,7 +3904,7 @@
       </c>
       <c r="AD11" s="1"/>
       <c r="AE11" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AF11" s="1"/>
       <c r="AG11" s="1" t="s">
@@ -3912,11 +3912,11 @@
       </c>
       <c r="AH11" s="1"/>
       <c r="AI11" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="AJ11" s="1"/>
       <c r="AK11" s="1" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="AL11" s="1"/>
       <c r="AM11" s="1" t="s">
@@ -3924,7 +3924,7 @@
       </c>
       <c r="AN11" s="1"/>
       <c r="AO11" s="1" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="AP11" s="1"/>
       <c r="AQ11" s="1" t="s">
@@ -4133,13 +4133,13 @@
         <v>19</v>
       </c>
       <c r="F16" s="10"/>
-      <c r="G16" s="10" t="s">
-        <v>22</v>
-      </c>
+      <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
+      <c r="K16" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
@@ -4232,17 +4232,17 @@
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F18" s="11"/>
-      <c r="G18" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H18" s="11"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
+      <c r="K18" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="L18" s="11"/>
       <c r="M18" s="12"/>
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
@@ -4280,20 +4280,20 @@
       <c r="A19" s="2"/>
       <c r="B19" s="1"/>
       <c r="C19" s="12" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="12" t="s">
         <v>21</v>
       </c>
       <c r="F19" s="12"/>
-      <c r="G19" s="12" t="s">
-        <v>46</v>
-      </c>
+      <c r="G19" s="12"/>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
+      <c r="K19" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
       <c r="N19" s="12"/>
@@ -4375,11 +4375,11 @@
         <v>53</v>
       </c>
       <c r="AH20" s="10"/>
-      <c r="AI20" s="10" t="s">
+      <c r="AI20" s="10"/>
+      <c r="AJ20" s="10"/>
+      <c r="AK20" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AJ20" s="10"/>
-      <c r="AK20" s="10"/>
       <c r="AL20" s="10"/>
       <c r="AM20" s="10"/>
       <c r="AN20" s="10"/>
@@ -4440,11 +4440,11 @@
       <c r="A22" s="2"/>
       <c r="B22" s="1"/>
       <c r="C22" s="11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="12"/>
@@ -4458,11 +4458,11 @@
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
       <c r="Q22" s="11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R22" s="11"/>
       <c r="S22" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="T22" s="11"/>
       <c r="U22" s="12"/>
@@ -4481,12 +4481,12 @@
         <v>71</v>
       </c>
       <c r="AH22" s="11"/>
-      <c r="AI22" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="AJ22" s="11"/>
-      <c r="AK22" s="12"/>
-      <c r="AL22" s="12"/>
+      <c r="AI22" s="12"/>
+      <c r="AJ22" s="12"/>
+      <c r="AK22" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL22" s="11"/>
       <c r="AM22" s="12"/>
       <c r="AN22" s="12"/>
       <c r="AO22" s="12"/>
@@ -4498,7 +4498,7 @@
       <c r="A23" s="2"/>
       <c r="B23" s="1"/>
       <c r="C23" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="12" t="s">
@@ -4516,11 +4516,11 @@
       <c r="O23" s="12"/>
       <c r="P23" s="12"/>
       <c r="Q23" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R23" s="12"/>
       <c r="S23" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="T23" s="12"/>
       <c r="U23" s="12"/>
@@ -4539,11 +4539,11 @@
         <v>21</v>
       </c>
       <c r="AH23" s="12"/>
-      <c r="AI23" s="12" t="s">
-        <v>42</v>
-      </c>
+      <c r="AI23" s="12"/>
       <c r="AJ23" s="12"/>
-      <c r="AK23" s="12"/>
+      <c r="AK23" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="AL23" s="12"/>
       <c r="AM23" s="12"/>
       <c r="AN23" s="12"/>
@@ -4563,11 +4563,11 @@
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
-      <c r="I24" s="10" t="s">
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
@@ -4587,9 +4587,7 @@
       <c r="Z24" s="10"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="10"/>
-      <c r="AC24" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="AC24" s="10"/>
       <c r="AD24" s="10"/>
       <c r="AE24" s="10"/>
       <c r="AF24" s="10"/>
@@ -4603,7 +4601,9 @@
         <v>30</v>
       </c>
       <c r="AN24" s="10"/>
-      <c r="AO24" s="10"/>
+      <c r="AO24" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="AP24" s="10"/>
       <c r="AQ24" s="1" t="s">
         <v>10</v>
@@ -4665,18 +4665,18 @@
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
-      <c r="I26" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="J26" s="11"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="L26" s="11"/>
       <c r="M26" s="12"/>
       <c r="N26" s="12"/>
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
       <c r="Q26" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R26" s="11"/>
       <c r="S26" s="12"/>
@@ -4689,10 +4689,8 @@
       <c r="Z26" s="12"/>
       <c r="AA26" s="12"/>
       <c r="AB26" s="12"/>
-      <c r="AC26" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD26" s="11"/>
+      <c r="AC26" s="12"/>
+      <c r="AD26" s="12"/>
       <c r="AE26" s="12"/>
       <c r="AF26" s="12"/>
       <c r="AG26" s="12"/>
@@ -4702,11 +4700,13 @@
       <c r="AK26" s="12"/>
       <c r="AL26" s="12"/>
       <c r="AM26" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="AN26" s="11"/>
-      <c r="AO26" s="12"/>
-      <c r="AP26" s="12"/>
+      <c r="AO26" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP26" s="11"/>
       <c r="AQ26" s="1"/>
       <c r="AR26" s="4"/>
     </row>
@@ -4719,18 +4719,18 @@
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
-      <c r="I27" s="12" t="s">
-        <v>56</v>
-      </c>
+      <c r="I27" s="12"/>
       <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
+      <c r="K27" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
       <c r="N27" s="12"/>
       <c r="O27" s="12"/>
       <c r="P27" s="12"/>
       <c r="Q27" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="R27" s="12"/>
       <c r="S27" s="12"/>
@@ -4743,9 +4743,7 @@
       <c r="Z27" s="12"/>
       <c r="AA27" s="12"/>
       <c r="AB27" s="12"/>
-      <c r="AC27" s="12" t="s">
-        <v>39</v>
-      </c>
+      <c r="AC27" s="12"/>
       <c r="AD27" s="12"/>
       <c r="AE27" s="12"/>
       <c r="AF27" s="12"/>
@@ -4756,10 +4754,12 @@
       <c r="AK27" s="12"/>
       <c r="AL27" s="12"/>
       <c r="AM27" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN27" s="12"/>
+      <c r="AO27" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AN27" s="12"/>
-      <c r="AO27" s="12"/>
       <c r="AP27" s="12"/>
       <c r="AQ27" s="1"/>
       <c r="AR27" s="4"/>
@@ -4959,23 +4959,23 @@
       <c r="B32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="10"/>
+      <c r="C32" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="D32" s="10"/>
-      <c r="E32" s="10" t="s">
-        <v>19</v>
-      </c>
+      <c r="E32" s="10"/>
       <c r="F32" s="10"/>
-      <c r="G32" s="10" t="s">
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
       <c r="J32" s="10"/>
-      <c r="K32" s="10" t="s">
-        <v>22</v>
-      </c>
+      <c r="K32" s="10"/>
       <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
+      <c r="M32" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="N32" s="10"/>
       <c r="O32" s="10"/>
       <c r="P32" s="10"/>
@@ -5061,24 +5061,24 @@
     <row r="34" spans="1:44" ht="20" customHeight="1">
       <c r="A34" s="2"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="H34" s="11"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="11" t="s">
+      <c r="C34" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="11"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="J34" s="11"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="L34" s="11"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
+      <c r="N34" s="11"/>
       <c r="O34" s="12"/>
       <c r="P34" s="12"/>
       <c r="Q34" s="12"/>
@@ -5113,23 +5113,23 @@
     <row r="35" spans="1:44" ht="20" customHeight="1">
       <c r="A35" s="2"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="12"/>
+      <c r="C35" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="D35" s="12"/>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
       <c r="N35" s="12"/>
       <c r="O35" s="12"/>
       <c r="P35" s="12"/>
@@ -5181,7 +5181,9 @@
       <c r="H36" s="10"/>
       <c r="I36" s="10"/>
       <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
+      <c r="K36" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="L36" s="10"/>
       <c r="M36" s="10"/>
       <c r="N36" s="10"/>
@@ -5215,11 +5217,11 @@
         <v>28</v>
       </c>
       <c r="AL36" s="10"/>
-      <c r="AM36" s="10" t="s">
+      <c r="AM36" s="10"/>
+      <c r="AN36" s="10"/>
+      <c r="AO36" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AN36" s="10"/>
-      <c r="AO36" s="10"/>
       <c r="AP36" s="10"/>
       <c r="AQ36" s="1" t="s">
         <v>9</v>
@@ -5276,27 +5278,29 @@
       <c r="A38" s="2"/>
       <c r="B38" s="1"/>
       <c r="C38" s="11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D38" s="11"/>
       <c r="E38" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F38" s="11"/>
       <c r="G38" s="11" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H38" s="11"/>
       <c r="I38" s="12"/>
       <c r="J38" s="12"/>
-      <c r="K38" s="12"/>
-      <c r="L38" s="12"/>
+      <c r="K38" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="L38" s="11"/>
       <c r="M38" s="12"/>
       <c r="N38" s="12"/>
       <c r="O38" s="12"/>
       <c r="P38" s="12"/>
       <c r="Q38" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R38" s="11"/>
       <c r="S38" s="12"/>
@@ -5316,19 +5320,19 @@
       <c r="AG38" s="12"/>
       <c r="AH38" s="12"/>
       <c r="AI38" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AJ38" s="11"/>
       <c r="AK38" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AL38" s="11"/>
-      <c r="AM38" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN38" s="11"/>
-      <c r="AO38" s="12"/>
-      <c r="AP38" s="12"/>
+      <c r="AM38" s="12"/>
+      <c r="AN38" s="12"/>
+      <c r="AO38" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP38" s="11"/>
       <c r="AQ38" s="1"/>
       <c r="AR38" s="4"/>
     </row>
@@ -5336,7 +5340,7 @@
       <c r="A39" s="2"/>
       <c r="B39" s="1"/>
       <c r="C39" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="12" t="s">
@@ -5344,19 +5348,21 @@
       </c>
       <c r="F39" s="12"/>
       <c r="G39" s="12" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H39" s="12"/>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
-      <c r="K39" s="12"/>
+      <c r="K39" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="L39" s="12"/>
       <c r="M39" s="12"/>
       <c r="N39" s="12"/>
       <c r="O39" s="12"/>
       <c r="P39" s="12"/>
       <c r="Q39" s="12" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="R39" s="12"/>
       <c r="S39" s="12"/>
@@ -5376,18 +5382,18 @@
       <c r="AG39" s="12"/>
       <c r="AH39" s="12"/>
       <c r="AI39" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AJ39" s="12"/>
       <c r="AK39" s="12" t="s">
         <v>42</v>
       </c>
       <c r="AL39" s="12"/>
-      <c r="AM39" s="12" t="s">
+      <c r="AM39" s="12"/>
+      <c r="AN39" s="12"/>
+      <c r="AO39" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="AN39" s="12"/>
-      <c r="AO39" s="12"/>
       <c r="AP39" s="12"/>
       <c r="AQ39" s="1"/>
       <c r="AR39" s="4"/>
@@ -5401,7 +5407,9 @@
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
+      <c r="G40" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
       <c r="J40" s="10"/>
@@ -5419,19 +5427,19 @@
       <c r="T40" s="10"/>
       <c r="U40" s="10"/>
       <c r="V40" s="10"/>
-      <c r="W40" s="10" t="s">
-        <v>49</v>
-      </c>
+      <c r="W40" s="10"/>
       <c r="X40" s="10"/>
       <c r="Y40" s="10"/>
       <c r="Z40" s="10"/>
-      <c r="AA40" s="10"/>
+      <c r="AA40" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="AB40" s="10"/>
-      <c r="AC40" s="10"/>
+      <c r="AC40" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="AD40" s="10"/>
-      <c r="AE40" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="AE40" s="10"/>
       <c r="AF40" s="10"/>
       <c r="AG40" s="10"/>
       <c r="AH40" s="10"/>
@@ -5439,9 +5447,7 @@
       <c r="AJ40" s="10"/>
       <c r="AK40" s="10"/>
       <c r="AL40" s="10"/>
-      <c r="AM40" s="10" t="s">
-        <v>30</v>
-      </c>
+      <c r="AM40" s="10"/>
       <c r="AN40" s="10"/>
       <c r="AO40" s="10"/>
       <c r="AP40" s="10"/>
@@ -5503,12 +5509,14 @@
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
+      <c r="G42" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H42" s="11"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
       <c r="K42" s="11" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L42" s="11"/>
       <c r="M42" s="12"/>
@@ -5521,30 +5529,28 @@
       <c r="T42" s="12"/>
       <c r="U42" s="12"/>
       <c r="V42" s="12"/>
-      <c r="W42" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="X42" s="11"/>
+      <c r="W42" s="12"/>
+      <c r="X42" s="12"/>
       <c r="Y42" s="12"/>
       <c r="Z42" s="12"/>
-      <c r="AA42" s="12"/>
-      <c r="AB42" s="12"/>
-      <c r="AC42" s="12"/>
-      <c r="AD42" s="12"/>
-      <c r="AE42" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF42" s="11"/>
+      <c r="AA42" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB42" s="11"/>
+      <c r="AC42" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD42" s="11"/>
+      <c r="AE42" s="12"/>
+      <c r="AF42" s="12"/>
       <c r="AG42" s="12"/>
       <c r="AH42" s="12"/>
       <c r="AI42" s="12"/>
       <c r="AJ42" s="12"/>
       <c r="AK42" s="12"/>
       <c r="AL42" s="12"/>
-      <c r="AM42" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="AN42" s="11"/>
+      <c r="AM42" s="12"/>
+      <c r="AN42" s="12"/>
       <c r="AO42" s="12"/>
       <c r="AP42" s="12"/>
       <c r="AQ42" s="1"/>
@@ -5557,12 +5563,14 @@
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
+      <c r="G43" s="12" t="s">
+        <v>45</v>
+      </c>
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
       <c r="K43" s="12" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="L43" s="12"/>
       <c r="M43" s="12"/>
@@ -5575,19 +5583,19 @@
       <c r="T43" s="12"/>
       <c r="U43" s="12"/>
       <c r="V43" s="12"/>
-      <c r="W43" s="12" t="s">
-        <v>44</v>
-      </c>
+      <c r="W43" s="12"/>
       <c r="X43" s="12"/>
       <c r="Y43" s="12"/>
       <c r="Z43" s="12"/>
-      <c r="AA43" s="12"/>
+      <c r="AA43" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="AB43" s="12"/>
-      <c r="AC43" s="12"/>
+      <c r="AC43" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="AD43" s="12"/>
-      <c r="AE43" s="12" t="s">
-        <v>39</v>
-      </c>
+      <c r="AE43" s="12"/>
       <c r="AF43" s="12"/>
       <c r="AG43" s="12"/>
       <c r="AH43" s="12"/>
@@ -5595,9 +5603,7 @@
       <c r="AJ43" s="12"/>
       <c r="AK43" s="12"/>
       <c r="AL43" s="12"/>
-      <c r="AM43" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="AM43" s="12"/>
       <c r="AN43" s="12"/>
       <c r="AO43" s="12"/>
       <c r="AP43" s="12"/>
@@ -5805,21 +5811,21 @@
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
-      <c r="I48" s="10"/>
+      <c r="I48" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
       <c r="L48" s="10"/>
-      <c r="M48" s="10" t="s">
-        <v>47</v>
-      </c>
+      <c r="M48" s="10"/>
       <c r="N48" s="10"/>
       <c r="O48" s="10"/>
       <c r="P48" s="10"/>
-      <c r="Q48" s="10"/>
+      <c r="Q48" s="10" t="s">
+        <v>24</v>
+      </c>
       <c r="R48" s="10"/>
-      <c r="S48" s="10" t="s">
-        <v>24</v>
-      </c>
+      <c r="S48" s="10"/>
       <c r="T48" s="10"/>
       <c r="U48" s="10"/>
       <c r="V48" s="10"/>
@@ -5835,11 +5841,11 @@
       <c r="AF48" s="10"/>
       <c r="AG48" s="10"/>
       <c r="AH48" s="10"/>
-      <c r="AI48" s="10"/>
+      <c r="AI48" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="AJ48" s="10"/>
-      <c r="AK48" s="10" t="s">
-        <v>28</v>
-      </c>
+      <c r="AK48" s="10"/>
       <c r="AL48" s="10"/>
       <c r="AM48" s="10"/>
       <c r="AN48" s="10"/>
@@ -5907,22 +5913,22 @@
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
       <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-      <c r="J50" s="12"/>
+      <c r="I50" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J50" s="11"/>
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
-      <c r="M50" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="N50" s="11"/>
+      <c r="M50" s="12"/>
+      <c r="N50" s="12"/>
       <c r="O50" s="12"/>
       <c r="P50" s="12"/>
-      <c r="Q50" s="12"/>
-      <c r="R50" s="12"/>
-      <c r="S50" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="T50" s="11"/>
+      <c r="Q50" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="R50" s="11"/>
+      <c r="S50" s="12"/>
+      <c r="T50" s="12"/>
       <c r="U50" s="12"/>
       <c r="V50" s="12"/>
       <c r="W50" s="12"/>
@@ -5937,12 +5943,12 @@
       <c r="AF50" s="12"/>
       <c r="AG50" s="12"/>
       <c r="AH50" s="12"/>
-      <c r="AI50" s="12"/>
-      <c r="AJ50" s="12"/>
-      <c r="AK50" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL50" s="11"/>
+      <c r="AI50" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ50" s="11"/>
+      <c r="AK50" s="12"/>
+      <c r="AL50" s="12"/>
       <c r="AM50" s="12"/>
       <c r="AN50" s="12"/>
       <c r="AO50" s="12"/>
@@ -5959,21 +5965,21 @@
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
       <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
+      <c r="I51" s="12" t="s">
+        <v>46</v>
+      </c>
       <c r="J51" s="12"/>
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
-      <c r="M51" s="12" t="s">
-        <v>46</v>
-      </c>
+      <c r="M51" s="12"/>
       <c r="N51" s="12"/>
       <c r="O51" s="12"/>
       <c r="P51" s="12"/>
-      <c r="Q51" s="12"/>
+      <c r="Q51" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="R51" s="12"/>
-      <c r="S51" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="S51" s="12"/>
       <c r="T51" s="12"/>
       <c r="U51" s="12"/>
       <c r="V51" s="12"/>
@@ -5989,11 +5995,11 @@
       <c r="AF51" s="12"/>
       <c r="AG51" s="12"/>
       <c r="AH51" s="12"/>
-      <c r="AI51" s="12"/>
+      <c r="AI51" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="AJ51" s="12"/>
-      <c r="AK51" s="12" t="s">
-        <v>60</v>
-      </c>
+      <c r="AK51" s="12"/>
       <c r="AL51" s="12"/>
       <c r="AM51" s="12"/>
       <c r="AN51" s="12"/>
@@ -6011,7 +6017,9 @@
         <v>19</v>
       </c>
       <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
+      <c r="E52" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="F52" s="10"/>
       <c r="G52" s="10" t="s">
         <v>22</v>
@@ -6037,9 +6045,7 @@
       <c r="V52" s="10"/>
       <c r="W52" s="10"/>
       <c r="X52" s="10"/>
-      <c r="Y52" s="10" t="s">
-        <v>51</v>
-      </c>
+      <c r="Y52" s="10"/>
       <c r="Z52" s="10"/>
       <c r="AA52" s="10" t="s">
         <v>51</v>
@@ -6051,11 +6057,11 @@
       <c r="AF52" s="10"/>
       <c r="AG52" s="10"/>
       <c r="AH52" s="10"/>
-      <c r="AI52" s="10" t="s">
+      <c r="AI52" s="10"/>
+      <c r="AJ52" s="10"/>
+      <c r="AK52" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AJ52" s="10"/>
-      <c r="AK52" s="10"/>
       <c r="AL52" s="10"/>
       <c r="AM52" s="10"/>
       <c r="AN52" s="10"/>
@@ -6116,21 +6122,23 @@
       <c r="A54" s="2"/>
       <c r="B54" s="1"/>
       <c r="C54" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D54" s="11"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
+      <c r="E54" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F54" s="11"/>
       <c r="G54" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H54" s="11"/>
       <c r="I54" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="J54" s="11"/>
       <c r="K54" s="11" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="L54" s="11"/>
       <c r="M54" s="12"/>
@@ -6145,12 +6153,10 @@
       <c r="V54" s="12"/>
       <c r="W54" s="12"/>
       <c r="X54" s="12"/>
-      <c r="Y54" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z54" s="11"/>
+      <c r="Y54" s="12"/>
+      <c r="Z54" s="12"/>
       <c r="AA54" s="11" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AB54" s="11"/>
       <c r="AC54" s="12"/>
@@ -6159,12 +6165,12 @@
       <c r="AF54" s="12"/>
       <c r="AG54" s="12"/>
       <c r="AH54" s="12"/>
-      <c r="AI54" s="11" t="s">
+      <c r="AI54" s="12"/>
+      <c r="AJ54" s="12"/>
+      <c r="AK54" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="AJ54" s="11"/>
-      <c r="AK54" s="12"/>
-      <c r="AL54" s="12"/>
+      <c r="AL54" s="11"/>
       <c r="AM54" s="12"/>
       <c r="AN54" s="12"/>
       <c r="AO54" s="12"/>
@@ -6176,21 +6182,23 @@
       <c r="A55" s="2"/>
       <c r="B55" s="1"/>
       <c r="C55" s="12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
+      <c r="E55" s="12" t="s">
+        <v>37</v>
+      </c>
       <c r="F55" s="12"/>
       <c r="G55" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H55" s="12"/>
       <c r="I55" s="12" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="J55" s="12"/>
       <c r="K55" s="12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="L55" s="12"/>
       <c r="M55" s="12"/>
@@ -6205,12 +6213,10 @@
       <c r="V55" s="12"/>
       <c r="W55" s="12"/>
       <c r="X55" s="12"/>
-      <c r="Y55" s="12" t="s">
-        <v>38</v>
-      </c>
+      <c r="Y55" s="12"/>
       <c r="Z55" s="12"/>
       <c r="AA55" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="AB55" s="12"/>
       <c r="AC55" s="12"/>
@@ -6219,11 +6225,11 @@
       <c r="AF55" s="12"/>
       <c r="AG55" s="12"/>
       <c r="AH55" s="12"/>
-      <c r="AI55" s="12" t="s">
-        <v>32</v>
-      </c>
+      <c r="AI55" s="12"/>
       <c r="AJ55" s="12"/>
-      <c r="AK55" s="12"/>
+      <c r="AK55" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="AL55" s="12"/>
       <c r="AM55" s="12"/>
       <c r="AN55" s="12"/>
@@ -6249,7 +6255,9 @@
         <v>22</v>
       </c>
       <c r="L56" s="10"/>
-      <c r="M56" s="10"/>
+      <c r="M56" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="N56" s="10"/>
       <c r="O56" s="10"/>
       <c r="P56" s="10"/>
@@ -6257,13 +6265,13 @@
       <c r="R56" s="10"/>
       <c r="S56" s="10"/>
       <c r="T56" s="10"/>
-      <c r="U56" s="10" t="s">
-        <v>49</v>
-      </c>
+      <c r="U56" s="10"/>
       <c r="V56" s="10"/>
       <c r="W56" s="10"/>
       <c r="X56" s="10"/>
-      <c r="Y56" s="10"/>
+      <c r="Y56" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="Z56" s="10"/>
       <c r="AA56" s="10"/>
       <c r="AB56" s="10"/>
@@ -6277,9 +6285,7 @@
       <c r="AJ56" s="10"/>
       <c r="AK56" s="10"/>
       <c r="AL56" s="10"/>
-      <c r="AM56" s="10" t="s">
-        <v>30</v>
-      </c>
+      <c r="AM56" s="10"/>
       <c r="AN56" s="10"/>
       <c r="AO56" s="10" t="s">
         <v>30</v>
@@ -6348,25 +6354,27 @@
       <c r="I58" s="12"/>
       <c r="J58" s="12"/>
       <c r="K58" s="11" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="L58" s="11"/>
-      <c r="M58" s="12"/>
-      <c r="N58" s="12"/>
+      <c r="M58" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="N58" s="11"/>
       <c r="O58" s="12"/>
       <c r="P58" s="12"/>
       <c r="Q58" s="12"/>
       <c r="R58" s="12"/>
       <c r="S58" s="12"/>
       <c r="T58" s="12"/>
-      <c r="U58" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="V58" s="11"/>
+      <c r="U58" s="12"/>
+      <c r="V58" s="12"/>
       <c r="W58" s="12"/>
       <c r="X58" s="12"/>
-      <c r="Y58" s="12"/>
-      <c r="Z58" s="12"/>
+      <c r="Y58" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z58" s="11"/>
       <c r="AA58" s="12"/>
       <c r="AB58" s="12"/>
       <c r="AC58" s="12"/>
@@ -6379,10 +6387,8 @@
       <c r="AJ58" s="12"/>
       <c r="AK58" s="12"/>
       <c r="AL58" s="12"/>
-      <c r="AM58" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="AN58" s="11"/>
+      <c r="AM58" s="12"/>
+      <c r="AN58" s="12"/>
       <c r="AO58" s="11" t="s">
         <v>65</v>
       </c>
@@ -6402,10 +6408,12 @@
       <c r="I59" s="12"/>
       <c r="J59" s="12"/>
       <c r="K59" s="12" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="L59" s="12"/>
-      <c r="M59" s="12"/>
+      <c r="M59" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="N59" s="12"/>
       <c r="O59" s="12"/>
       <c r="P59" s="12"/>
@@ -6413,13 +6421,13 @@
       <c r="R59" s="12"/>
       <c r="S59" s="12"/>
       <c r="T59" s="12"/>
-      <c r="U59" s="12" t="s">
-        <v>44</v>
-      </c>
+      <c r="U59" s="12"/>
       <c r="V59" s="12"/>
       <c r="W59" s="12"/>
       <c r="X59" s="12"/>
-      <c r="Y59" s="12"/>
+      <c r="Y59" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="Z59" s="12"/>
       <c r="AA59" s="12"/>
       <c r="AB59" s="12"/>
@@ -6433,12 +6441,10 @@
       <c r="AJ59" s="12"/>
       <c r="AK59" s="12"/>
       <c r="AL59" s="12"/>
-      <c r="AM59" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="AM59" s="12"/>
       <c r="AN59" s="12"/>
       <c r="AO59" s="12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="AP59" s="12"/>
       <c r="AQ59" s="1"/>
@@ -6760,19 +6766,19 @@
       <c r="S66" s="12"/>
       <c r="T66" s="12"/>
       <c r="U66" s="11" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="V66" s="11"/>
       <c r="W66" s="12"/>
       <c r="X66" s="12"/>
       <c r="Y66" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z66" s="11"/>
       <c r="AA66" s="12"/>
       <c r="AB66" s="12"/>
       <c r="AC66" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD66" s="11"/>
       <c r="AE66" s="12"/>
@@ -6818,7 +6824,7 @@
       <c r="W67" s="12"/>
       <c r="X67" s="12"/>
       <c r="Y67" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Z67" s="12"/>
       <c r="AA67" s="12"/>
@@ -6851,7 +6857,9 @@
         <v>19</v>
       </c>
       <c r="D68" s="10"/>
-      <c r="E68" s="10"/>
+      <c r="E68" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="F68" s="10"/>
       <c r="G68" s="10" t="s">
         <v>22</v>
@@ -6881,7 +6889,9 @@
       <c r="X68" s="10"/>
       <c r="Y68" s="10"/>
       <c r="Z68" s="10"/>
-      <c r="AA68" s="10"/>
+      <c r="AA68" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="AB68" s="10"/>
       <c r="AC68" s="10"/>
       <c r="AD68" s="10"/>
@@ -6952,27 +6962,29 @@
       <c r="A70" s="2"/>
       <c r="B70" s="1"/>
       <c r="C70" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D70" s="11"/>
-      <c r="E70" s="12"/>
-      <c r="F70" s="12"/>
+      <c r="E70" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F70" s="11"/>
       <c r="G70" s="11" t="s">
         <v>63</v>
       </c>
       <c r="H70" s="11"/>
       <c r="I70" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="J70" s="11"/>
       <c r="K70" s="11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L70" s="11"/>
       <c r="M70" s="12"/>
       <c r="N70" s="12"/>
       <c r="O70" s="11" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="P70" s="11"/>
       <c r="Q70" s="12"/>
@@ -6985,8 +6997,10 @@
       <c r="X70" s="12"/>
       <c r="Y70" s="12"/>
       <c r="Z70" s="12"/>
-      <c r="AA70" s="12"/>
-      <c r="AB70" s="12"/>
+      <c r="AA70" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB70" s="11"/>
       <c r="AC70" s="12"/>
       <c r="AD70" s="12"/>
       <c r="AE70" s="12"/>
@@ -7011,24 +7025,26 @@
         <v>32</v>
       </c>
       <c r="D71" s="12"/>
-      <c r="E71" s="12"/>
+      <c r="E71" s="12" t="s">
+        <v>37</v>
+      </c>
       <c r="F71" s="12"/>
       <c r="G71" s="12" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="H71" s="12"/>
       <c r="I71" s="12" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="J71" s="12"/>
       <c r="K71" s="12" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="L71" s="12"/>
       <c r="M71" s="12"/>
       <c r="N71" s="12"/>
       <c r="O71" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P71" s="12"/>
       <c r="Q71" s="12"/>
@@ -7041,7 +7057,9 @@
       <c r="X71" s="12"/>
       <c r="Y71" s="12"/>
       <c r="Z71" s="12"/>
-      <c r="AA71" s="12"/>
+      <c r="AA71" s="12" t="s">
+        <v>39</v>
+      </c>
       <c r="AB71" s="12"/>
       <c r="AC71" s="12"/>
       <c r="AD71" s="12"/>
@@ -7085,11 +7103,11 @@
       <c r="T72" s="10"/>
       <c r="U72" s="10"/>
       <c r="V72" s="10"/>
-      <c r="W72" s="10"/>
+      <c r="W72" s="10" t="s">
+        <v>49</v>
+      </c>
       <c r="X72" s="10"/>
-      <c r="Y72" s="10" t="s">
-        <v>51</v>
-      </c>
+      <c r="Y72" s="10"/>
       <c r="Z72" s="10"/>
       <c r="AA72" s="10"/>
       <c r="AB72" s="10"/>
@@ -7105,9 +7123,7 @@
       <c r="AL72" s="10"/>
       <c r="AM72" s="10"/>
       <c r="AN72" s="10"/>
-      <c r="AO72" s="10" t="s">
-        <v>30</v>
-      </c>
+      <c r="AO72" s="10"/>
       <c r="AP72" s="10"/>
       <c r="AQ72" s="1" t="s">
         <v>10</v>
@@ -7183,12 +7199,12 @@
       <c r="T74" s="12"/>
       <c r="U74" s="12"/>
       <c r="V74" s="12"/>
-      <c r="W74" s="12"/>
-      <c r="X74" s="12"/>
-      <c r="Y74" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z74" s="11"/>
+      <c r="W74" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="X74" s="11"/>
+      <c r="Y74" s="12"/>
+      <c r="Z74" s="12"/>
       <c r="AA74" s="12"/>
       <c r="AB74" s="12"/>
       <c r="AC74" s="12"/>
@@ -7203,10 +7219,8 @@
       <c r="AL74" s="12"/>
       <c r="AM74" s="12"/>
       <c r="AN74" s="12"/>
-      <c r="AO74" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="AP74" s="11"/>
+      <c r="AO74" s="12"/>
+      <c r="AP74" s="12"/>
       <c r="AQ74" s="1"/>
       <c r="AR74" s="4"/>
     </row>
@@ -7233,11 +7247,11 @@
       <c r="T75" s="12"/>
       <c r="U75" s="12"/>
       <c r="V75" s="12"/>
-      <c r="W75" s="12"/>
+      <c r="W75" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="X75" s="12"/>
-      <c r="Y75" s="12" t="s">
-        <v>39</v>
-      </c>
+      <c r="Y75" s="12"/>
       <c r="Z75" s="12"/>
       <c r="AA75" s="12"/>
       <c r="AB75" s="12"/>
@@ -7253,9 +7267,7 @@
       <c r="AL75" s="12"/>
       <c r="AM75" s="12"/>
       <c r="AN75" s="12"/>
-      <c r="AO75" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="AO75" s="12"/>
       <c r="AP75" s="12"/>
       <c r="AQ75" s="1"/>
       <c r="AR75" s="4"/>
@@ -7481,11 +7493,11 @@
       <c r="V80" s="10"/>
       <c r="W80" s="10"/>
       <c r="X80" s="10"/>
-      <c r="Y80" s="10" t="s">
+      <c r="Y80" s="10"/>
+      <c r="Z80" s="10"/>
+      <c r="AA80" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="Z80" s="10"/>
-      <c r="AA80" s="10"/>
       <c r="AB80" s="10"/>
       <c r="AC80" s="10"/>
       <c r="AD80" s="10"/>
@@ -7562,11 +7574,11 @@
       <c r="A82" s="2"/>
       <c r="B82" s="1"/>
       <c r="C82" s="11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D82" s="11"/>
       <c r="E82" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F82" s="11"/>
       <c r="G82" s="12"/>
@@ -7587,12 +7599,12 @@
       <c r="V82" s="12"/>
       <c r="W82" s="12"/>
       <c r="X82" s="12"/>
-      <c r="Y82" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z82" s="11"/>
-      <c r="AA82" s="12"/>
-      <c r="AB82" s="12"/>
+      <c r="Y82" s="12"/>
+      <c r="Z82" s="12"/>
+      <c r="AA82" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB82" s="11"/>
       <c r="AC82" s="12"/>
       <c r="AD82" s="12"/>
       <c r="AE82" s="12"/>
@@ -7600,7 +7612,7 @@
       <c r="AG82" s="12"/>
       <c r="AH82" s="12"/>
       <c r="AI82" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AJ82" s="11"/>
       <c r="AK82" s="11" t="s">
@@ -7618,11 +7630,11 @@
       <c r="A83" s="2"/>
       <c r="B83" s="1"/>
       <c r="C83" s="12" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D83" s="12"/>
       <c r="E83" s="12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F83" s="12"/>
       <c r="G83" s="12"/>
@@ -7643,11 +7655,11 @@
       <c r="V83" s="12"/>
       <c r="W83" s="12"/>
       <c r="X83" s="12"/>
-      <c r="Y83" s="12" t="s">
+      <c r="Y83" s="12"/>
+      <c r="Z83" s="12"/>
+      <c r="AA83" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="Z83" s="12"/>
-      <c r="AA83" s="12"/>
       <c r="AB83" s="12"/>
       <c r="AC83" s="12"/>
       <c r="AD83" s="12"/>
@@ -7656,11 +7668,11 @@
       <c r="AG83" s="12"/>
       <c r="AH83" s="12"/>
       <c r="AI83" s="12" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="AJ83" s="12"/>
       <c r="AK83" s="12" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="AL83" s="12"/>
       <c r="AM83" s="12"/>
@@ -7675,15 +7687,11 @@
       <c r="B84" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C84" s="10" t="s">
-        <v>19</v>
-      </c>
+      <c r="C84" s="10"/>
       <c r="D84" s="10"/>
       <c r="E84" s="10"/>
       <c r="F84" s="10"/>
-      <c r="G84" s="10" t="s">
-        <v>22</v>
-      </c>
+      <c r="G84" s="10"/>
       <c r="H84" s="10"/>
       <c r="I84" s="10"/>
       <c r="J84" s="10"/>
@@ -7691,13 +7699,13 @@
         <v>22</v>
       </c>
       <c r="L84" s="10"/>
-      <c r="M84" s="10" t="s">
-        <v>47</v>
-      </c>
+      <c r="M84" s="10"/>
       <c r="N84" s="10"/>
       <c r="O84" s="10"/>
       <c r="P84" s="10"/>
-      <c r="Q84" s="10"/>
+      <c r="Q84" s="10" t="s">
+        <v>24</v>
+      </c>
       <c r="R84" s="10"/>
       <c r="S84" s="10" t="s">
         <v>24</v>
@@ -7705,7 +7713,9 @@
       <c r="T84" s="10"/>
       <c r="U84" s="10"/>
       <c r="V84" s="10"/>
-      <c r="W84" s="10"/>
+      <c r="W84" s="10" t="s">
+        <v>49</v>
+      </c>
       <c r="X84" s="10"/>
       <c r="Y84" s="10"/>
       <c r="Z84" s="10"/>
@@ -7779,38 +7789,36 @@
     <row r="86" spans="1:44" ht="20" customHeight="1">
       <c r="A86" s="2"/>
       <c r="B86" s="1"/>
-      <c r="C86" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D86" s="11"/>
+      <c r="C86" s="12"/>
+      <c r="D86" s="12"/>
       <c r="E86" s="12"/>
       <c r="F86" s="12"/>
-      <c r="G86" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="H86" s="11"/>
+      <c r="G86" s="12"/>
+      <c r="H86" s="12"/>
       <c r="I86" s="12"/>
       <c r="J86" s="12"/>
       <c r="K86" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L86" s="11"/>
-      <c r="M86" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="N86" s="11"/>
+      <c r="M86" s="12"/>
+      <c r="N86" s="12"/>
       <c r="O86" s="12"/>
       <c r="P86" s="12"/>
-      <c r="Q86" s="12"/>
-      <c r="R86" s="12"/>
+      <c r="Q86" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="R86" s="11"/>
       <c r="S86" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="T86" s="11"/>
       <c r="U86" s="12"/>
       <c r="V86" s="12"/>
-      <c r="W86" s="12"/>
-      <c r="X86" s="12"/>
+      <c r="W86" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="X86" s="11"/>
       <c r="Y86" s="12"/>
       <c r="Z86" s="12"/>
       <c r="AA86" s="12"/>
@@ -7835,29 +7843,25 @@
     <row r="87" spans="1:44" ht="20" customHeight="1">
       <c r="A87" s="2"/>
       <c r="B87" s="1"/>
-      <c r="C87" s="12" t="s">
-        <v>32</v>
-      </c>
+      <c r="C87" s="12"/>
       <c r="D87" s="12"/>
       <c r="E87" s="12"/>
       <c r="F87" s="12"/>
-      <c r="G87" s="12" t="s">
-        <v>39</v>
-      </c>
+      <c r="G87" s="12"/>
       <c r="H87" s="12"/>
       <c r="I87" s="12"/>
       <c r="J87" s="12"/>
       <c r="K87" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L87" s="12"/>
-      <c r="M87" s="12" t="s">
-        <v>56</v>
-      </c>
+      <c r="M87" s="12"/>
       <c r="N87" s="12"/>
       <c r="O87" s="12"/>
       <c r="P87" s="12"/>
-      <c r="Q87" s="12"/>
+      <c r="Q87" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="R87" s="12"/>
       <c r="S87" s="12" t="s">
         <v>34</v>
@@ -7865,7 +7869,9 @@
       <c r="T87" s="12"/>
       <c r="U87" s="12"/>
       <c r="V87" s="12"/>
-      <c r="W87" s="12"/>
+      <c r="W87" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="X87" s="12"/>
       <c r="Y87" s="12"/>
       <c r="Z87" s="12"/>
@@ -7915,9 +7921,7 @@
       <c r="V88" s="10"/>
       <c r="W88" s="10"/>
       <c r="X88" s="10"/>
-      <c r="Y88" s="10" t="s">
-        <v>51</v>
-      </c>
+      <c r="Y88" s="10"/>
       <c r="Z88" s="10"/>
       <c r="AA88" s="10"/>
       <c r="AB88" s="10"/>
@@ -7933,7 +7937,9 @@
       <c r="AL88" s="10"/>
       <c r="AM88" s="10"/>
       <c r="AN88" s="10"/>
-      <c r="AO88" s="10"/>
+      <c r="AO88" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="AP88" s="10"/>
       <c r="AQ88" s="1" t="s">
         <v>10</v>
@@ -8011,10 +8017,8 @@
       <c r="V90" s="12"/>
       <c r="W90" s="12"/>
       <c r="X90" s="12"/>
-      <c r="Y90" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z90" s="11"/>
+      <c r="Y90" s="12"/>
+      <c r="Z90" s="12"/>
       <c r="AA90" s="12"/>
       <c r="AB90" s="12"/>
       <c r="AC90" s="12"/>
@@ -8029,8 +8033,10 @@
       <c r="AL90" s="12"/>
       <c r="AM90" s="12"/>
       <c r="AN90" s="12"/>
-      <c r="AO90" s="12"/>
-      <c r="AP90" s="12"/>
+      <c r="AO90" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP90" s="11"/>
       <c r="AQ90" s="1"/>
       <c r="AR90" s="4"/>
     </row>
@@ -8059,9 +8065,7 @@
       <c r="V91" s="12"/>
       <c r="W91" s="12"/>
       <c r="X91" s="12"/>
-      <c r="Y91" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="Y91" s="12"/>
       <c r="Z91" s="12"/>
       <c r="AA91" s="12"/>
       <c r="AB91" s="12"/>
@@ -8077,7 +8081,9 @@
       <c r="AL91" s="12"/>
       <c r="AM91" s="12"/>
       <c r="AN91" s="12"/>
-      <c r="AO91" s="12"/>
+      <c r="AO91" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="AP91" s="12"/>
       <c r="AQ91" s="1"/>
       <c r="AR91" s="4"/>
@@ -8416,7 +8422,7 @@
       <c r="AK98" s="12"/>
       <c r="AL98" s="12"/>
       <c r="AM98" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AN98" s="11"/>
       <c r="AO98" s="12"/>
@@ -8479,17 +8485,13 @@
       <c r="B100" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C100" s="10" t="s">
-        <v>19</v>
-      </c>
+      <c r="C100" s="10"/>
       <c r="D100" s="10"/>
       <c r="E100" s="10"/>
       <c r="F100" s="10"/>
       <c r="G100" s="10"/>
       <c r="H100" s="10"/>
-      <c r="I100" s="10" t="s">
-        <v>22</v>
-      </c>
+      <c r="I100" s="10"/>
       <c r="J100" s="10"/>
       <c r="K100" s="10" t="s">
         <v>22</v>
@@ -8499,9 +8501,7 @@
       <c r="N100" s="10"/>
       <c r="O100" s="10"/>
       <c r="P100" s="10"/>
-      <c r="Q100" s="10" t="s">
-        <v>24</v>
-      </c>
+      <c r="Q100" s="10"/>
       <c r="R100" s="10"/>
       <c r="S100" s="10"/>
       <c r="T100" s="10"/>
@@ -8517,7 +8517,9 @@
         <v>26</v>
       </c>
       <c r="AD100" s="10"/>
-      <c r="AE100" s="10"/>
+      <c r="AE100" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="AF100" s="10"/>
       <c r="AG100" s="10"/>
       <c r="AH100" s="10"/>
@@ -8527,7 +8529,9 @@
       <c r="AL100" s="10"/>
       <c r="AM100" s="10"/>
       <c r="AN100" s="10"/>
-      <c r="AO100" s="10"/>
+      <c r="AO100" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="AP100" s="10"/>
       <c r="AQ100" s="1" t="s">
         <v>9</v>
@@ -8583,30 +8587,24 @@
     <row r="102" spans="1:44" ht="20" customHeight="1">
       <c r="A102" s="2"/>
       <c r="B102" s="1"/>
-      <c r="C102" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D102" s="11"/>
+      <c r="C102" s="12"/>
+      <c r="D102" s="12"/>
       <c r="E102" s="12"/>
       <c r="F102" s="12"/>
       <c r="G102" s="12"/>
       <c r="H102" s="12"/>
-      <c r="I102" s="11" t="s">
+      <c r="I102" s="12"/>
+      <c r="J102" s="12"/>
+      <c r="K102" s="11" t="s">
         <v>65</v>
-      </c>
-      <c r="J102" s="11"/>
-      <c r="K102" s="11" t="s">
-        <v>64</v>
       </c>
       <c r="L102" s="11"/>
       <c r="M102" s="12"/>
       <c r="N102" s="12"/>
       <c r="O102" s="12"/>
       <c r="P102" s="12"/>
-      <c r="Q102" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="R102" s="11"/>
+      <c r="Q102" s="12"/>
+      <c r="R102" s="12"/>
       <c r="S102" s="12"/>
       <c r="T102" s="12"/>
       <c r="U102" s="12"/>
@@ -8618,11 +8616,13 @@
       <c r="AA102" s="12"/>
       <c r="AB102" s="12"/>
       <c r="AC102" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AD102" s="11"/>
-      <c r="AE102" s="12"/>
-      <c r="AF102" s="12"/>
+      <c r="AE102" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF102" s="11"/>
       <c r="AG102" s="12"/>
       <c r="AH102" s="12"/>
       <c r="AI102" s="12"/>
@@ -8631,37 +8631,33 @@
       <c r="AL102" s="12"/>
       <c r="AM102" s="12"/>
       <c r="AN102" s="12"/>
-      <c r="AO102" s="12"/>
-      <c r="AP102" s="12"/>
+      <c r="AO102" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP102" s="11"/>
       <c r="AQ102" s="1"/>
       <c r="AR102" s="4"/>
     </row>
     <row r="103" spans="1:44" ht="20" customHeight="1">
       <c r="A103" s="2"/>
       <c r="B103" s="1"/>
-      <c r="C103" s="12" t="s">
-        <v>32</v>
-      </c>
+      <c r="C103" s="12"/>
       <c r="D103" s="12"/>
       <c r="E103" s="12"/>
       <c r="F103" s="12"/>
       <c r="G103" s="12"/>
       <c r="H103" s="12"/>
-      <c r="I103" s="12" t="s">
-        <v>56</v>
-      </c>
+      <c r="I103" s="12"/>
       <c r="J103" s="12"/>
       <c r="K103" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L103" s="12"/>
       <c r="M103" s="12"/>
       <c r="N103" s="12"/>
       <c r="O103" s="12"/>
       <c r="P103" s="12"/>
-      <c r="Q103" s="12" t="s">
-        <v>39</v>
-      </c>
+      <c r="Q103" s="12"/>
       <c r="R103" s="12"/>
       <c r="S103" s="12"/>
       <c r="T103" s="12"/>
@@ -8677,7 +8673,9 @@
         <v>34</v>
       </c>
       <c r="AD103" s="12"/>
-      <c r="AE103" s="12"/>
+      <c r="AE103" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="AF103" s="12"/>
       <c r="AG103" s="12"/>
       <c r="AH103" s="12"/>
@@ -8687,7 +8685,9 @@
       <c r="AL103" s="12"/>
       <c r="AM103" s="12"/>
       <c r="AN103" s="12"/>
-      <c r="AO103" s="12"/>
+      <c r="AO103" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="AP103" s="12"/>
       <c r="AQ103" s="1"/>
       <c r="AR103" s="4"/>
@@ -9158,7 +9158,8 @@
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C32:D33"/>
-    <mergeCell ref="C34:D35"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
     <mergeCell ref="C48:D49"/>
     <mergeCell ref="C50:D51"/>
     <mergeCell ref="C64:D65"/>
@@ -9181,11 +9182,9 @@
     <mergeCell ref="C70:D70"/>
     <mergeCell ref="C71:D71"/>
     <mergeCell ref="C84:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C86:D87"/>
     <mergeCell ref="C100:D101"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C102:D103"/>
     <mergeCell ref="C24:D25"/>
     <mergeCell ref="C26:D27"/>
     <mergeCell ref="C40:D41"/>
@@ -9214,8 +9213,7 @@
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E32:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E34:F35"/>
     <mergeCell ref="E48:F49"/>
     <mergeCell ref="E50:F51"/>
     <mergeCell ref="E64:F65"/>
@@ -9232,9 +9230,11 @@
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="E52:F53"/>
-    <mergeCell ref="E54:F55"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E55:F55"/>
     <mergeCell ref="E68:F69"/>
-    <mergeCell ref="E70:F71"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="E71:F71"/>
     <mergeCell ref="E84:F85"/>
     <mergeCell ref="E86:F87"/>
     <mergeCell ref="E100:F101"/>
@@ -9264,11 +9264,9 @@
     <mergeCell ref="E108:F109"/>
     <mergeCell ref="E110:F111"/>
     <mergeCell ref="G16:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G18:H19"/>
     <mergeCell ref="G32:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G34:H35"/>
     <mergeCell ref="G48:H49"/>
     <mergeCell ref="G50:H51"/>
     <mergeCell ref="G64:H65"/>
@@ -9289,14 +9287,14 @@
     <mergeCell ref="G70:H70"/>
     <mergeCell ref="G71:H71"/>
     <mergeCell ref="G84:H85"/>
-    <mergeCell ref="G86:H86"/>
-    <mergeCell ref="G87:H87"/>
+    <mergeCell ref="G86:H87"/>
     <mergeCell ref="G100:H101"/>
     <mergeCell ref="G102:H103"/>
     <mergeCell ref="G24:H25"/>
     <mergeCell ref="G26:H27"/>
     <mergeCell ref="G40:H41"/>
-    <mergeCell ref="G42:H43"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G43:H43"/>
     <mergeCell ref="G56:H57"/>
     <mergeCell ref="G58:H59"/>
     <mergeCell ref="G72:H73"/>
@@ -9320,9 +9318,11 @@
     <mergeCell ref="I16:J17"/>
     <mergeCell ref="I18:J19"/>
     <mergeCell ref="I32:J33"/>
-    <mergeCell ref="I34:J35"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="I35:J35"/>
     <mergeCell ref="I48:J49"/>
-    <mergeCell ref="I50:J51"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="I51:J51"/>
     <mergeCell ref="I64:J65"/>
     <mergeCell ref="I66:J67"/>
     <mergeCell ref="I80:J81"/>
@@ -9342,11 +9342,9 @@
     <mergeCell ref="I84:J85"/>
     <mergeCell ref="I86:J87"/>
     <mergeCell ref="I100:J101"/>
-    <mergeCell ref="I102:J102"/>
-    <mergeCell ref="I103:J103"/>
+    <mergeCell ref="I102:J103"/>
     <mergeCell ref="I24:J25"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I26:J27"/>
     <mergeCell ref="I40:J41"/>
     <mergeCell ref="I42:J43"/>
     <mergeCell ref="I56:J57"/>
@@ -9370,10 +9368,10 @@
     <mergeCell ref="I108:J109"/>
     <mergeCell ref="I110:J111"/>
     <mergeCell ref="K16:L17"/>
-    <mergeCell ref="K18:L19"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
     <mergeCell ref="K32:L33"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="K34:L35"/>
     <mergeCell ref="K48:L49"/>
     <mergeCell ref="K50:L51"/>
     <mergeCell ref="K64:L65"/>
@@ -9385,7 +9383,8 @@
     <mergeCell ref="K20:L21"/>
     <mergeCell ref="K22:L23"/>
     <mergeCell ref="K36:L37"/>
-    <mergeCell ref="K38:L39"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="K39:L39"/>
     <mergeCell ref="K52:L53"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K55:L55"/>
@@ -9399,7 +9398,8 @@
     <mergeCell ref="K102:L102"/>
     <mergeCell ref="K103:L103"/>
     <mergeCell ref="K24:L25"/>
-    <mergeCell ref="K26:L27"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K27:L27"/>
     <mergeCell ref="K40:L41"/>
     <mergeCell ref="K42:L42"/>
     <mergeCell ref="K43:L43"/>
@@ -9427,10 +9427,10 @@
     <mergeCell ref="M16:N17"/>
     <mergeCell ref="M18:N19"/>
     <mergeCell ref="M32:N33"/>
-    <mergeCell ref="M34:N35"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="M35:N35"/>
     <mergeCell ref="M48:N49"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="M51:N51"/>
+    <mergeCell ref="M50:N51"/>
     <mergeCell ref="M64:N65"/>
     <mergeCell ref="M66:N67"/>
     <mergeCell ref="M80:N81"/>
@@ -9446,8 +9446,7 @@
     <mergeCell ref="M68:N69"/>
     <mergeCell ref="M70:N71"/>
     <mergeCell ref="M84:N85"/>
-    <mergeCell ref="M86:N86"/>
-    <mergeCell ref="M87:N87"/>
+    <mergeCell ref="M86:N87"/>
     <mergeCell ref="M100:N101"/>
     <mergeCell ref="M102:N103"/>
     <mergeCell ref="M24:N25"/>
@@ -9455,7 +9454,8 @@
     <mergeCell ref="M40:N41"/>
     <mergeCell ref="M42:N43"/>
     <mergeCell ref="M56:N57"/>
-    <mergeCell ref="M58:N59"/>
+    <mergeCell ref="M58:N58"/>
+    <mergeCell ref="M59:N59"/>
     <mergeCell ref="M72:N73"/>
     <mergeCell ref="M74:N75"/>
     <mergeCell ref="M88:N89"/>
@@ -9528,7 +9528,8 @@
     <mergeCell ref="Q32:R33"/>
     <mergeCell ref="Q34:R35"/>
     <mergeCell ref="Q48:R49"/>
-    <mergeCell ref="Q50:R51"/>
+    <mergeCell ref="Q50:R50"/>
+    <mergeCell ref="Q51:R51"/>
     <mergeCell ref="Q64:R65"/>
     <mergeCell ref="Q66:R67"/>
     <mergeCell ref="Q80:R81"/>
@@ -9546,10 +9547,10 @@
     <mergeCell ref="Q68:R69"/>
     <mergeCell ref="Q70:R71"/>
     <mergeCell ref="Q84:R85"/>
-    <mergeCell ref="Q86:R87"/>
+    <mergeCell ref="Q86:R86"/>
+    <mergeCell ref="Q87:R87"/>
     <mergeCell ref="Q100:R101"/>
-    <mergeCell ref="Q102:R102"/>
-    <mergeCell ref="Q103:R103"/>
+    <mergeCell ref="Q102:R103"/>
     <mergeCell ref="Q24:R25"/>
     <mergeCell ref="Q26:R26"/>
     <mergeCell ref="Q27:R27"/>
@@ -9580,8 +9581,7 @@
     <mergeCell ref="S32:T33"/>
     <mergeCell ref="S34:T35"/>
     <mergeCell ref="S48:T49"/>
-    <mergeCell ref="S50:T50"/>
-    <mergeCell ref="S51:T51"/>
+    <mergeCell ref="S50:T51"/>
     <mergeCell ref="S64:T65"/>
     <mergeCell ref="S66:T67"/>
     <mergeCell ref="S80:T81"/>
@@ -9656,8 +9656,7 @@
     <mergeCell ref="U40:V41"/>
     <mergeCell ref="U42:V43"/>
     <mergeCell ref="U56:V57"/>
-    <mergeCell ref="U58:V58"/>
-    <mergeCell ref="U59:V59"/>
+    <mergeCell ref="U58:V59"/>
     <mergeCell ref="U72:V73"/>
     <mergeCell ref="U74:V75"/>
     <mergeCell ref="U88:V89"/>
@@ -9697,18 +9696,19 @@
     <mergeCell ref="W68:X69"/>
     <mergeCell ref="W70:X71"/>
     <mergeCell ref="W84:X85"/>
-    <mergeCell ref="W86:X87"/>
+    <mergeCell ref="W86:X86"/>
+    <mergeCell ref="W87:X87"/>
     <mergeCell ref="W100:X101"/>
     <mergeCell ref="W102:X103"/>
     <mergeCell ref="W24:X25"/>
     <mergeCell ref="W26:X27"/>
     <mergeCell ref="W40:X41"/>
-    <mergeCell ref="W42:X42"/>
-    <mergeCell ref="W43:X43"/>
+    <mergeCell ref="W42:X43"/>
     <mergeCell ref="W56:X57"/>
     <mergeCell ref="W58:X59"/>
     <mergeCell ref="W72:X73"/>
-    <mergeCell ref="W74:X75"/>
+    <mergeCell ref="W74:X74"/>
+    <mergeCell ref="W75:X75"/>
     <mergeCell ref="W88:X89"/>
     <mergeCell ref="W90:X91"/>
     <mergeCell ref="W104:X105"/>
@@ -9735,8 +9735,7 @@
     <mergeCell ref="Y66:Z66"/>
     <mergeCell ref="Y67:Z67"/>
     <mergeCell ref="Y80:Z81"/>
-    <mergeCell ref="Y82:Z82"/>
-    <mergeCell ref="Y83:Z83"/>
+    <mergeCell ref="Y82:Z83"/>
     <mergeCell ref="Y96:Z97"/>
     <mergeCell ref="Y98:Z99"/>
     <mergeCell ref="Y20:Z21"/>
@@ -9744,8 +9743,7 @@
     <mergeCell ref="Y36:Z37"/>
     <mergeCell ref="Y38:Z39"/>
     <mergeCell ref="Y52:Z53"/>
-    <mergeCell ref="Y54:Z54"/>
-    <mergeCell ref="Y55:Z55"/>
+    <mergeCell ref="Y54:Z55"/>
     <mergeCell ref="Y68:Z69"/>
     <mergeCell ref="Y70:Z71"/>
     <mergeCell ref="Y84:Z85"/>
@@ -9757,13 +9755,12 @@
     <mergeCell ref="Y40:Z41"/>
     <mergeCell ref="Y42:Z43"/>
     <mergeCell ref="Y56:Z57"/>
-    <mergeCell ref="Y58:Z59"/>
+    <mergeCell ref="Y58:Z58"/>
+    <mergeCell ref="Y59:Z59"/>
     <mergeCell ref="Y72:Z73"/>
-    <mergeCell ref="Y74:Z74"/>
-    <mergeCell ref="Y75:Z75"/>
+    <mergeCell ref="Y74:Z75"/>
     <mergeCell ref="Y88:Z89"/>
-    <mergeCell ref="Y90:Z90"/>
-    <mergeCell ref="Y91:Z91"/>
+    <mergeCell ref="Y90:Z91"/>
     <mergeCell ref="Y104:Z105"/>
     <mergeCell ref="Y106:Z107"/>
     <mergeCell ref="Y28:Z29"/>
@@ -9787,7 +9784,8 @@
     <mergeCell ref="AA64:AB65"/>
     <mergeCell ref="AA66:AB67"/>
     <mergeCell ref="AA80:AB81"/>
-    <mergeCell ref="AA82:AB83"/>
+    <mergeCell ref="AA82:AB82"/>
+    <mergeCell ref="AA83:AB83"/>
     <mergeCell ref="AA96:AB97"/>
     <mergeCell ref="AA98:AB99"/>
     <mergeCell ref="AA20:AB21"/>
@@ -9798,7 +9796,8 @@
     <mergeCell ref="AA54:AB54"/>
     <mergeCell ref="AA55:AB55"/>
     <mergeCell ref="AA68:AB69"/>
-    <mergeCell ref="AA70:AB71"/>
+    <mergeCell ref="AA70:AB70"/>
+    <mergeCell ref="AA71:AB71"/>
     <mergeCell ref="AA84:AB85"/>
     <mergeCell ref="AA86:AB87"/>
     <mergeCell ref="AA100:AB101"/>
@@ -9806,7 +9805,8 @@
     <mergeCell ref="AA24:AB25"/>
     <mergeCell ref="AA26:AB27"/>
     <mergeCell ref="AA40:AB41"/>
-    <mergeCell ref="AA42:AB43"/>
+    <mergeCell ref="AA42:AB42"/>
+    <mergeCell ref="AA43:AB43"/>
     <mergeCell ref="AA56:AB57"/>
     <mergeCell ref="AA58:AB59"/>
     <mergeCell ref="AA72:AB73"/>
@@ -9854,10 +9854,10 @@
     <mergeCell ref="AC102:AD102"/>
     <mergeCell ref="AC103:AD103"/>
     <mergeCell ref="AC24:AD25"/>
-    <mergeCell ref="AC26:AD26"/>
-    <mergeCell ref="AC27:AD27"/>
+    <mergeCell ref="AC26:AD27"/>
     <mergeCell ref="AC40:AD41"/>
-    <mergeCell ref="AC42:AD43"/>
+    <mergeCell ref="AC42:AD42"/>
+    <mergeCell ref="AC43:AD43"/>
     <mergeCell ref="AC56:AD57"/>
     <mergeCell ref="AC58:AD59"/>
     <mergeCell ref="AC72:AD73"/>
@@ -9901,12 +9901,12 @@
     <mergeCell ref="AE84:AF85"/>
     <mergeCell ref="AE86:AF87"/>
     <mergeCell ref="AE100:AF101"/>
-    <mergeCell ref="AE102:AF103"/>
+    <mergeCell ref="AE102:AF102"/>
+    <mergeCell ref="AE103:AF103"/>
     <mergeCell ref="AE24:AF25"/>
     <mergeCell ref="AE26:AF27"/>
     <mergeCell ref="AE40:AF41"/>
-    <mergeCell ref="AE42:AF42"/>
-    <mergeCell ref="AE43:AF43"/>
+    <mergeCell ref="AE42:AF43"/>
     <mergeCell ref="AE56:AF57"/>
     <mergeCell ref="AE58:AF59"/>
     <mergeCell ref="AE72:AF73"/>
@@ -9982,7 +9982,8 @@
     <mergeCell ref="AI32:AJ33"/>
     <mergeCell ref="AI34:AJ35"/>
     <mergeCell ref="AI48:AJ49"/>
-    <mergeCell ref="AI50:AJ51"/>
+    <mergeCell ref="AI50:AJ50"/>
+    <mergeCell ref="AI51:AJ51"/>
     <mergeCell ref="AI64:AJ65"/>
     <mergeCell ref="AI66:AJ67"/>
     <mergeCell ref="AI80:AJ81"/>
@@ -9991,14 +9992,12 @@
     <mergeCell ref="AI96:AJ97"/>
     <mergeCell ref="AI98:AJ99"/>
     <mergeCell ref="AI20:AJ21"/>
-    <mergeCell ref="AI22:AJ22"/>
-    <mergeCell ref="AI23:AJ23"/>
+    <mergeCell ref="AI22:AJ23"/>
     <mergeCell ref="AI36:AJ37"/>
     <mergeCell ref="AI38:AJ38"/>
     <mergeCell ref="AI39:AJ39"/>
     <mergeCell ref="AI52:AJ53"/>
-    <mergeCell ref="AI54:AJ54"/>
-    <mergeCell ref="AI55:AJ55"/>
+    <mergeCell ref="AI54:AJ55"/>
     <mergeCell ref="AI68:AJ69"/>
     <mergeCell ref="AI70:AJ71"/>
     <mergeCell ref="AI84:AJ85"/>
@@ -10034,8 +10033,7 @@
     <mergeCell ref="AK32:AL33"/>
     <mergeCell ref="AK34:AL35"/>
     <mergeCell ref="AK48:AL49"/>
-    <mergeCell ref="AK50:AL50"/>
-    <mergeCell ref="AK51:AL51"/>
+    <mergeCell ref="AK50:AL51"/>
     <mergeCell ref="AK64:AL65"/>
     <mergeCell ref="AK66:AL67"/>
     <mergeCell ref="AK80:AL81"/>
@@ -10044,12 +10042,14 @@
     <mergeCell ref="AK96:AL97"/>
     <mergeCell ref="AK98:AL99"/>
     <mergeCell ref="AK20:AL21"/>
-    <mergeCell ref="AK22:AL23"/>
+    <mergeCell ref="AK22:AL22"/>
+    <mergeCell ref="AK23:AL23"/>
     <mergeCell ref="AK36:AL37"/>
     <mergeCell ref="AK38:AL38"/>
     <mergeCell ref="AK39:AL39"/>
     <mergeCell ref="AK52:AL53"/>
-    <mergeCell ref="AK54:AL55"/>
+    <mergeCell ref="AK54:AL54"/>
+    <mergeCell ref="AK55:AL55"/>
     <mergeCell ref="AK68:AL69"/>
     <mergeCell ref="AK70:AL71"/>
     <mergeCell ref="AK84:AL85"/>
@@ -10096,8 +10096,7 @@
     <mergeCell ref="AM20:AN21"/>
     <mergeCell ref="AM22:AN23"/>
     <mergeCell ref="AM36:AN37"/>
-    <mergeCell ref="AM38:AN38"/>
-    <mergeCell ref="AM39:AN39"/>
+    <mergeCell ref="AM38:AN39"/>
     <mergeCell ref="AM52:AN53"/>
     <mergeCell ref="AM54:AN55"/>
     <mergeCell ref="AM68:AN69"/>
@@ -10110,11 +10109,9 @@
     <mergeCell ref="AM26:AN26"/>
     <mergeCell ref="AM27:AN27"/>
     <mergeCell ref="AM40:AN41"/>
-    <mergeCell ref="AM42:AN42"/>
-    <mergeCell ref="AM43:AN43"/>
+    <mergeCell ref="AM42:AN43"/>
     <mergeCell ref="AM56:AN57"/>
-    <mergeCell ref="AM58:AN58"/>
-    <mergeCell ref="AM59:AN59"/>
+    <mergeCell ref="AM58:AN59"/>
     <mergeCell ref="AM72:AN73"/>
     <mergeCell ref="AM74:AN75"/>
     <mergeCell ref="AM88:AN89"/>
@@ -10148,7 +10145,8 @@
     <mergeCell ref="AO20:AP21"/>
     <mergeCell ref="AO22:AP23"/>
     <mergeCell ref="AO36:AP37"/>
-    <mergeCell ref="AO38:AP39"/>
+    <mergeCell ref="AO38:AP38"/>
+    <mergeCell ref="AO39:AP39"/>
     <mergeCell ref="AO52:AP53"/>
     <mergeCell ref="AO54:AP55"/>
     <mergeCell ref="AO68:AP69"/>
@@ -10156,19 +10154,21 @@
     <mergeCell ref="AO84:AP85"/>
     <mergeCell ref="AO86:AP87"/>
     <mergeCell ref="AO100:AP101"/>
-    <mergeCell ref="AO102:AP103"/>
+    <mergeCell ref="AO102:AP102"/>
+    <mergeCell ref="AO103:AP103"/>
     <mergeCell ref="AO24:AP25"/>
-    <mergeCell ref="AO26:AP27"/>
+    <mergeCell ref="AO26:AP26"/>
+    <mergeCell ref="AO27:AP27"/>
     <mergeCell ref="AO40:AP41"/>
     <mergeCell ref="AO42:AP43"/>
     <mergeCell ref="AO56:AP57"/>
     <mergeCell ref="AO58:AP58"/>
     <mergeCell ref="AO59:AP59"/>
     <mergeCell ref="AO72:AP73"/>
-    <mergeCell ref="AO74:AP74"/>
-    <mergeCell ref="AO75:AP75"/>
+    <mergeCell ref="AO74:AP75"/>
     <mergeCell ref="AO88:AP89"/>
-    <mergeCell ref="AO90:AP91"/>
+    <mergeCell ref="AO90:AP90"/>
+    <mergeCell ref="AO91:AP91"/>
     <mergeCell ref="AO104:AP105"/>
     <mergeCell ref="AO106:AP107"/>
     <mergeCell ref="AO28:AP29"/>

</xml_diff>